<commit_message>
DM-406: [DM-409] fix some responsiveness for practice show view
+ starting timeline styling
+ added scope for acts as list items that belong to practice
</commit_message>
<xml_diff>
--- a/lib/assets/Diffusion Marketplace.back.xlsx
+++ b/lib/assets/Diffusion Marketplace.back.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="584">
   <si>
     <t>Respondent ID</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Which of the following statements regarding Partners apply to this Practice? (Mark all that apply)</t>
   </si>
   <si>
-    <t>Please provide your best estimate rating of your Practice with regards to Impact on health/care experience on a scale of 1 - 4.</t>
-  </si>
-  <si>
     <t>What is the primary risk to implementation? Please describe how you would mitigate it.</t>
   </si>
   <si>
@@ -94,7 +91,19 @@
     <t>Please provide your best estimate of the Cost to Implement your Practice on a scale of 1 - 4</t>
   </si>
   <si>
-    <t>Please provide your best estimate of the Difficulty of Implementation your Practice on a scale of 1 - 4</t>
+    <t>Please provide your best estimate of the Complexity of Implementation of your Practice on a scale of 1 - 4 (Complexity of getting the practice started.)</t>
+  </si>
+  <si>
+    <t>Please provide your best estimate of the Complexity of Maintenance and Sustainability of your Practice on a scale of 1 - 4</t>
+  </si>
+  <si>
+    <t>Number of Departments required to implement the practice?</t>
+  </si>
+  <si>
+    <t>Is Information Technology (IT) required to implement the practice?</t>
+  </si>
+  <si>
+    <t>Is this practice a New Clinical Approach or New Process? Or is this practice a process change of something already being done? (Choose one of the following.)</t>
   </si>
   <si>
     <t>What job titles are required to implement this Practice?</t>
@@ -124,7 +133,7 @@
     <t>Will a new license or certification be required?</t>
   </si>
   <si>
-    <t>Under the side navigation "Origin" tab, please provide a photo of the individual who initiated the practice.</t>
+    <t>Please provide a photo of the individual who initiated the practice. (This will be displayed under "Origin of the practice")</t>
   </si>
   <si>
     <t>Please enter a 10-20 word title for the origin story of this Practice</t>
@@ -885,6 +894,129 @@
     <t>Publication Link 3</t>
   </si>
   <si>
+    <t>152.133.7.64</t>
+  </si>
+  <si>
+    <t>Susan.Hastings@va.gov</t>
+  </si>
+  <si>
+    <t>ashley.choate@va.gov</t>
+  </si>
+  <si>
+    <t>Getting Hospitalized Veterans Back on Their Feet: The STRIDE Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRIDE consists of a one-time gait and balance assessment conducted by a physical therapist, followed by daily supervised walks by a therapy or nursing assistant for the duration of the hospital stay. Program evaluation has demonstrated high satisfaction among Veteran participants and reduced need for post-acute institutional care.  </t>
+  </si>
+  <si>
+    <t>Immobility during hospitalization is a key contributor to hospital-associated disability. Fewer than 5% of hospitalized patients have physician orders for bed rest, yet hospitalized older adults spend only 4% of their time standing or walking. Older Veterans are especially vulnerable to the adverse physical effects of immobility and their resultant consequences. The hazards of immobility in the hospital have been recognized for more than 2 decades, but there are currently no VA-system wide approaches to address this important gap in clinical care. STRIDE is a supervised walking program for hospitalized older adults designed to address immobility during hospitalization and its negative consequences.</t>
+  </si>
+  <si>
+    <t>Susan N. Hastings, MD, MHSc, Director, Center of Innovation (COIN) for Health Services Research in Primary Care</t>
+  </si>
+  <si>
+    <t>Ashley Choate, MPH, Research Health Science Specialist</t>
+  </si>
+  <si>
+    <t>Elizabeth Mahanna, MPH, Research Health Science Specialist</t>
+  </si>
+  <si>
+    <t>John Bartle, STRIDE PT</t>
+  </si>
+  <si>
+    <t>02/01/2012</t>
+  </si>
+  <si>
+    <t>2. Initial Diffusion - The practice is undergoing active spread to other facilities with a footprint of less than 20% of all VA facilities or other defined target market.</t>
+  </si>
+  <si>
+    <t>3 months</t>
+  </si>
+  <si>
+    <t>Geriatrics and Extended Care; Mentoring Partnership Program</t>
+  </si>
+  <si>
+    <t>Role clarity among providers preparing to implement STRIDE</t>
+  </si>
+  <si>
+    <t>Designating key staff as champions, regularly educating referring providers and new staff about the program, and having assigned walkers helps to avoid the program decreasing in value after its initiation.</t>
+  </si>
+  <si>
+    <t>2. $10,000 - $50,000</t>
+  </si>
+  <si>
+    <t>2. Some complexity</t>
+  </si>
+  <si>
+    <t>2. Two departments</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>New Clinical Approach or New Process</t>
+  </si>
+  <si>
+    <t>Physical Therapist</t>
+  </si>
+  <si>
+    <t>Mobility Assistant (PTA, RN, CNA, Health Tech)</t>
+  </si>
+  <si>
+    <t>Permanent (partial FTE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobility equipment (such as gait belts, pedometers, stopwatches, walkers, safe lifting equipment) </t>
+  </si>
+  <si>
+    <t>Mobility Assistant</t>
+  </si>
+  <si>
+    <t>20 minutes</t>
+  </si>
+  <si>
+    <t>1 20 minute in person training to ensure ability to ambulate patients safely</t>
+  </si>
+  <si>
+    <t>competency checklist</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Ural and Vet Walking.jpg</t>
+  </si>
+  <si>
+    <t>Veteran and Mobilty Assistant Walking (Durham VA)</t>
+  </si>
+  <si>
+    <t>John and Vet-back-facing-Durham.png</t>
+  </si>
+  <si>
+    <t>STRIDE PT completing the initial gait assessment (Durham VA)</t>
+  </si>
+  <si>
+    <t>Vet-amputee-alone-Durham.png</t>
+  </si>
+  <si>
+    <t>Veteran out of bed walking with the STRIDE program</t>
+  </si>
+  <si>
+    <t>susan.hastings@va.gov</t>
+  </si>
+  <si>
+    <t>Susan N. Hastings \ Director, Center of Innovation (COIN) for Health Services Research in Primary Care</t>
+  </si>
+  <si>
+    <t>Ashley Choate \ Research Health Science Specialist</t>
+  </si>
+  <si>
+    <t>Elizabeth Mahanna \ Research Health Science Specialist</t>
+  </si>
+  <si>
+    <t>Outlook picture.jpg</t>
+  </si>
+  <si>
     <t>152.130.7.135</t>
   </si>
   <si>
@@ -912,18 +1044,9 @@
     <t>06/01/2018</t>
   </si>
   <si>
-    <t>2. Initial Diffusion - The practice is undergoing active spread to other facilities with a footprint of less than 20% of all VA facilities or other defined target market.</t>
-  </si>
-  <si>
-    <t>3 months</t>
-  </si>
-  <si>
     <t>Pay for Success project in VACO.</t>
   </si>
   <si>
-    <t>4. High or large Impact</t>
-  </si>
-  <si>
     <t>Lack of support within the PTSD treatment team to adopt IPS.</t>
   </si>
   <si>
@@ -945,9 +1068,6 @@
     <t>3. $50,000 - $250,000</t>
   </si>
   <si>
-    <t>2. Some difficulty to implement</t>
-  </si>
-  <si>
     <t>ACOS of Mental Health (existing employee)</t>
   </si>
   <si>
@@ -996,9 +1116,6 @@
     <t>IPS Supervision and Fidelity Monitoring (Toscano) Travel costs.</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Dr. Davis (2 of 4) (002).jpg</t>
   </si>
   <si>
@@ -1080,9 +1197,6 @@
     <t>6 months</t>
   </si>
   <si>
-    <t>3. Significant Impact</t>
-  </si>
-  <si>
     <t>Inadequate staffing.</t>
   </si>
   <si>
@@ -1101,10 +1215,7 @@
     <t>Hire the right person. Find volunteers with good writing skills and train them.</t>
   </si>
   <si>
-    <t>2. $10,000 - $50,000</t>
-  </si>
-  <si>
-    <t>3. Significant difficulty to implement</t>
+    <t>3. Significant complexity</t>
   </si>
   <si>
     <t>Writer-Editor (GS9)</t>
@@ -1503,7 +1614,7 @@
     <t>1. $0 - $10,000</t>
   </si>
   <si>
-    <t>1. Little to no difficulty to implement</t>
+    <t>1. Little to no complexity</t>
   </si>
   <si>
     <t>Diffusion Specialist</t>
@@ -1739,7 +1850,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="334" width="8.71"/>
+    <col customWidth="1" min="1" max="337" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1829,18 +1940,18 @@
       <c r="AN1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AT1" s="1"/>
       <c r="AU1" s="1" t="s">
         <v>26</v>
       </c>
@@ -1850,63 +1961,63 @@
       <c r="AW1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AX1" s="1"/>
-      <c r="AY1" s="1"/>
-      <c r="AZ1" s="1"/>
+      <c r="AX1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="BA1" s="1"/>
-      <c r="BB1" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="BB1" s="1"/>
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
+      <c r="BE1" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="BF1" s="1"/>
-      <c r="BG1" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="BG1" s="1"/>
       <c r="BH1" s="1"/>
       <c r="BI1" s="1"/>
-      <c r="BJ1" s="1"/>
+      <c r="BJ1" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="BK1" s="1"/>
-      <c r="BL1" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="BL1" s="1"/>
       <c r="BM1" s="1"/>
       <c r="BN1" s="1"/>
-      <c r="BO1" s="1"/>
+      <c r="BO1" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="BP1" s="1"/>
-      <c r="BQ1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="BQ1" s="1"/>
+      <c r="BR1" s="1"/>
       <c r="BS1" s="1"/>
-      <c r="BT1" s="1"/>
-      <c r="BU1" s="1"/>
+      <c r="BT1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="BV1" s="1"/>
-      <c r="BW1" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="BW1" s="1"/>
       <c r="BX1" s="1"/>
       <c r="BY1" s="1"/>
       <c r="BZ1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="CA1" s="1"/>
       <c r="CB1" s="1"/>
-      <c r="CC1" s="1"/>
+      <c r="CC1" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="CD1" s="1"/>
       <c r="CE1" s="1"/>
-      <c r="CF1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="CH1" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="CF1" s="1"/>
+      <c r="CG1" s="1"/>
+      <c r="CH1" s="1"/>
       <c r="CI1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1926,36 +2037,36 @@
         <v>44</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="CP1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="CR1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="CQ1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="CR1" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="CS1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="CT1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="CU1" s="1"/>
-      <c r="CV1" s="1"/>
-      <c r="CW1" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="CW1" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="CX1" s="1"/>
-      <c r="CY1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="CZ1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="DA1" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="CY1" s="1"/>
+      <c r="CZ1" s="1"/>
+      <c r="DA1" s="1"/>
       <c r="DB1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1965,16 +2076,22 @@
       <c r="DD1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="DE1" s="1"/>
-      <c r="DF1" s="1"/>
-      <c r="DG1" s="1"/>
+      <c r="DE1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="DH1" s="1"/>
-      <c r="DI1" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="DI1" s="1"/>
       <c r="DJ1" s="1"/>
       <c r="DK1" s="1"/>
-      <c r="DL1" s="1"/>
+      <c r="DL1" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="DM1" s="1"/>
       <c r="DN1" s="1"/>
       <c r="DO1" s="1"/>
@@ -1984,12 +2101,12 @@
       <c r="DS1" s="1"/>
       <c r="DT1" s="1"/>
       <c r="DU1" s="1"/>
-      <c r="DV1" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="DV1" s="1"/>
       <c r="DW1" s="1"/>
       <c r="DX1" s="1"/>
-      <c r="DY1" s="1"/>
+      <c r="DY1" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="DZ1" s="1"/>
       <c r="EA1" s="1"/>
       <c r="EB1" s="1"/>
@@ -2019,12 +2136,12 @@
       <c r="EZ1" s="1"/>
       <c r="FA1" s="1"/>
       <c r="FB1" s="1"/>
-      <c r="FC1" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="FC1" s="1"/>
       <c r="FD1" s="1"/>
       <c r="FE1" s="1"/>
-      <c r="FF1" s="1"/>
+      <c r="FF1" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="FG1" s="1"/>
       <c r="FH1" s="1"/>
       <c r="FI1" s="1"/>
@@ -2044,12 +2161,12 @@
       <c r="FW1" s="1"/>
       <c r="FX1" s="1"/>
       <c r="FY1" s="1"/>
-      <c r="FZ1" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="FZ1" s="1"/>
       <c r="GA1" s="1"/>
       <c r="GB1" s="1"/>
-      <c r="GC1" s="1"/>
+      <c r="GC1" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="GD1" s="1"/>
       <c r="GE1" s="1"/>
       <c r="GF1" s="1"/>
@@ -2060,29 +2177,29 @@
       <c r="GK1" s="1"/>
       <c r="GL1" s="1"/>
       <c r="GM1" s="1"/>
-      <c r="GN1" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="GN1" s="1"/>
       <c r="GO1" s="1"/>
       <c r="GP1" s="1"/>
-      <c r="GQ1" s="1"/>
+      <c r="GQ1" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="GR1" s="1"/>
       <c r="GS1" s="1"/>
       <c r="GT1" s="1"/>
       <c r="GU1" s="1"/>
-      <c r="GV1" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="GV1" s="1"/>
       <c r="GW1" s="1"/>
       <c r="GX1" s="1"/>
-      <c r="GY1" s="1"/>
+      <c r="GY1" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="GZ1" s="1"/>
-      <c r="HA1" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="HA1" s="1"/>
       <c r="HB1" s="1"/>
       <c r="HC1" s="1"/>
-      <c r="HD1" s="1"/>
+      <c r="HD1" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="HE1" s="1"/>
       <c r="HF1" s="1"/>
       <c r="HG1" s="1"/>
@@ -2115,12 +2232,12 @@
       <c r="IH1" s="1"/>
       <c r="II1" s="1"/>
       <c r="IJ1" s="1"/>
-      <c r="IK1" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="IK1" s="1"/>
       <c r="IL1" s="1"/>
       <c r="IM1" s="1"/>
-      <c r="IN1" s="1"/>
+      <c r="IN1" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="IO1" s="1"/>
       <c r="IP1" s="1"/>
       <c r="IQ1" s="1"/>
@@ -2129,12 +2246,12 @@
       <c r="IT1" s="1"/>
       <c r="IU1" s="1"/>
       <c r="IV1" s="1"/>
-      <c r="IW1" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="IW1" s="1"/>
       <c r="IX1" s="1"/>
       <c r="IY1" s="1"/>
-      <c r="IZ1" s="1"/>
+      <c r="IZ1" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="JA1" s="1"/>
       <c r="JB1" s="1"/>
       <c r="JC1" s="1"/>
@@ -2181,12 +2298,12 @@
       <c r="KR1" s="1"/>
       <c r="KS1" s="1"/>
       <c r="KT1" s="1"/>
-      <c r="KU1" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="KU1" s="1"/>
       <c r="KV1" s="1"/>
       <c r="KW1" s="1"/>
-      <c r="KX1" s="1"/>
+      <c r="KX1" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="KY1" s="1"/>
       <c r="KZ1" s="1"/>
       <c r="LA1" s="1"/>
@@ -2194,15 +2311,9 @@
       <c r="LC1" s="1"/>
       <c r="LD1" s="1"/>
       <c r="LE1" s="1"/>
-      <c r="LF1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="LG1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="LH1" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="LF1" s="1"/>
+      <c r="LG1" s="1"/>
+      <c r="LH1" s="1"/>
       <c r="LI1" s="1" t="s">
         <v>68</v>
       </c>
@@ -2227,19 +2338,28 @@
       <c r="LP1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="LQ1" s="1"/>
-      <c r="LR1" s="1"/>
+      <c r="LQ1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="LR1" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="LS1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="LT1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="LU1" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="LT1" s="1"/>
+      <c r="LU1" s="1"/>
       <c r="LV1" s="1" t="s">
         <v>79</v>
+      </c>
+      <c r="LW1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="LX1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="LY1" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2">
@@ -2253,130 +2373,130 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="V2" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="AB2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AT2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AC2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="AU2" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="AZ2" s="1" t="s">
         <v>106</v>
@@ -2430,16 +2550,16 @@
         <v>122</v>
       </c>
       <c r="BQ2" s="1" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="BR2" s="1" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="BS2" s="1" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="BT2" s="1" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="BU2" s="1" t="s">
         <v>106</v>
@@ -2448,13 +2568,13 @@
         <v>107</v>
       </c>
       <c r="BW2" s="1" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="BX2" s="1" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="BY2" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="BZ2" s="1" t="s">
         <v>126</v>
@@ -2475,52 +2595,52 @@
         <v>131</v>
       </c>
       <c r="CF2" s="1" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="CG2" s="1" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="CH2" s="1" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="CI2" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="CJ2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="CK2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="CL2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="CM2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="CN2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="CO2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="CP2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="CQ2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="CR2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="CS2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="CT2" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="CU2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="CV2" s="1" t="s">
         <v>83</v>
@@ -2532,28 +2652,28 @@
         <v>85</v>
       </c>
       <c r="CY2" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="CZ2" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="DA2" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="DB2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="DC2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="DD2" s="1" t="s">
-        <v>132</v>
+        <v>83</v>
       </c>
       <c r="DE2" s="1" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="DF2" s="1" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="DG2" s="1" t="s">
         <v>135</v>
@@ -2592,22 +2712,22 @@
         <v>146</v>
       </c>
       <c r="DS2" s="1" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="DT2" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="DU2" s="1" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="DV2" s="1" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="DW2" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="DX2" s="1" t="s">
-        <v>150</v>
+        <v>91</v>
       </c>
       <c r="DY2" s="1" t="s">
         <v>151</v>
@@ -2694,37 +2814,37 @@
         <v>178</v>
       </c>
       <c r="FA2" s="1" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="FB2" s="1" t="s">
-        <v>88</v>
+        <v>180</v>
       </c>
       <c r="FC2" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="FD2" s="1" t="s">
-        <v>180</v>
+        <v>102</v>
       </c>
       <c r="FE2" s="1" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="FF2" s="1" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="FG2" s="1" t="s">
-        <v>156</v>
+        <v>183</v>
       </c>
       <c r="FH2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="FI2" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="FI2" s="1" t="s">
+      <c r="FJ2" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="FJ2" s="1" t="s">
+      <c r="FK2" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="FK2" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="FL2" s="1" t="s">
         <v>162</v>
@@ -2733,16 +2853,16 @@
         <v>163</v>
       </c>
       <c r="FN2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="FO2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="FP2" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="FO2" s="1" t="s">
+      <c r="FQ2" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="FP2" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="FQ2" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="FR2" s="1" t="s">
         <v>172</v>
@@ -2754,70 +2874,70 @@
         <v>174</v>
       </c>
       <c r="FU2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="FV2" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="FV2" s="1" t="s">
+      <c r="FW2" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="FW2" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="FX2" s="1" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="FY2" s="1" t="s">
-        <v>88</v>
+        <v>180</v>
       </c>
       <c r="FZ2" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="GA2" s="1" t="s">
-        <v>183</v>
+        <v>102</v>
       </c>
       <c r="GB2" s="1" t="s">
-        <v>184</v>
+        <v>91</v>
       </c>
       <c r="GC2" s="1" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="GD2" s="1" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="GE2" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="GF2" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="GF2" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="GG2" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="GH2" s="1" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="GI2" s="1" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="GJ2" s="1" t="s">
         <v>177</v>
       </c>
       <c r="GK2" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="GL2" s="1" t="s">
-        <v>99</v>
+        <v>189</v>
       </c>
       <c r="GM2" s="1" t="s">
-        <v>88</v>
+        <v>180</v>
       </c>
       <c r="GN2" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="GO2" s="1" t="s">
-        <v>189</v>
+        <v>102</v>
       </c>
       <c r="GP2" s="1" t="s">
-        <v>190</v>
+        <v>91</v>
       </c>
       <c r="GQ2" s="1" t="s">
         <v>191</v>
@@ -2826,40 +2946,40 @@
         <v>192</v>
       </c>
       <c r="GS2" s="1" t="s">
-        <v>99</v>
+        <v>193</v>
       </c>
       <c r="GT2" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="GU2" s="1" t="s">
-        <v>88</v>
+        <v>195</v>
       </c>
       <c r="GV2" s="1" t="s">
-        <v>194</v>
+        <v>102</v>
       </c>
       <c r="GW2" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="GX2" s="1" t="s">
-        <v>194</v>
+        <v>91</v>
       </c>
       <c r="GY2" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="GZ2" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="HA2" s="1" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="HB2" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="HC2" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="HD2" s="1" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="HE2" s="1" t="s">
         <v>198</v>
@@ -2934,16 +3054,16 @@
         <v>221</v>
       </c>
       <c r="IC2" s="1" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="ID2" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="IE2" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="IF2" s="1" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="IG2" s="1" t="s">
         <v>225</v>
@@ -2955,16 +3075,16 @@
         <v>227</v>
       </c>
       <c r="IJ2" s="1" t="s">
-        <v>99</v>
+        <v>228</v>
       </c>
       <c r="IK2" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="IL2" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="IM2" s="1" t="s">
-        <v>230</v>
+        <v>102</v>
       </c>
       <c r="IN2" s="1" t="s">
         <v>231</v>
@@ -2973,34 +3093,34 @@
         <v>232</v>
       </c>
       <c r="IP2" s="1" t="s">
-        <v>170</v>
+        <v>233</v>
       </c>
       <c r="IQ2" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="IR2" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="IS2" s="1" t="s">
-        <v>235</v>
+        <v>173</v>
       </c>
       <c r="IT2" s="1" t="s">
-        <v>99</v>
+        <v>236</v>
       </c>
       <c r="IU2" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="IV2" s="1" t="s">
-        <v>88</v>
+        <v>238</v>
       </c>
       <c r="IW2" s="1" t="s">
-        <v>237</v>
+        <v>102</v>
       </c>
       <c r="IX2" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="IY2" s="1" t="s">
-        <v>239</v>
+        <v>91</v>
       </c>
       <c r="IZ2" s="1" t="s">
         <v>240</v>
@@ -3054,25 +3174,25 @@
         <v>256</v>
       </c>
       <c r="JQ2" s="1" t="s">
-        <v>185</v>
+        <v>257</v>
       </c>
       <c r="JR2" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="JS2" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="JT2" s="1" t="s">
-        <v>253</v>
+        <v>188</v>
       </c>
       <c r="JU2" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="JV2" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="JW2" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="JX2" s="1" t="s">
         <v>262</v>
@@ -3096,61 +3216,61 @@
         <v>268</v>
       </c>
       <c r="KE2" s="1" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="KF2" s="1" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="KG2" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="KH2" s="1" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="KI2" s="1" t="s">
-        <v>231</v>
+        <v>260</v>
       </c>
       <c r="KJ2" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="KK2" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="KL2" s="1" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="KM2" s="1" t="s">
         <v>274</v>
       </c>
       <c r="KN2" s="1" t="s">
-        <v>170</v>
+        <v>275</v>
       </c>
       <c r="KO2" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="KP2" s="1" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="KQ2" s="1" t="s">
-        <v>276</v>
+        <v>173</v>
       </c>
       <c r="KR2" s="1" t="s">
-        <v>99</v>
+        <v>278</v>
       </c>
       <c r="KS2" s="1" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="KT2" s="1" t="s">
-        <v>88</v>
+        <v>279</v>
       </c>
       <c r="KU2" s="1" t="s">
-        <v>278</v>
+        <v>102</v>
       </c>
       <c r="KV2" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="KW2" s="1" t="s">
-        <v>280</v>
+        <v>91</v>
       </c>
       <c r="KX2" s="1" t="s">
         <v>281</v>
@@ -3168,156 +3288,159 @@
         <v>285</v>
       </c>
       <c r="LC2" s="1" t="s">
-        <v>99</v>
+        <v>286</v>
       </c>
       <c r="LD2" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="LE2" s="1" t="s">
-        <v>88</v>
+        <v>288</v>
       </c>
       <c r="LF2" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="LG2" s="1" t="s">
-        <v>80</v>
+        <v>289</v>
       </c>
       <c r="LH2" s="1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="LI2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="LJ2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="LK2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="LL2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="LM2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="LN2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="LO2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="LP2" s="1" t="s">
-        <v>287</v>
+        <v>83</v>
       </c>
       <c r="LQ2" s="1" t="s">
-        <v>288</v>
+        <v>83</v>
       </c>
       <c r="LR2" s="1" t="s">
-        <v>289</v>
+        <v>83</v>
       </c>
       <c r="LS2" s="1" t="s">
-        <v>80</v>
+        <v>290</v>
       </c>
       <c r="LT2" s="1" t="s">
-        <v>80</v>
+        <v>291</v>
       </c>
       <c r="LU2" s="1" t="s">
-        <v>80</v>
+        <v>292</v>
       </c>
       <c r="LV2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
+      </c>
+      <c r="LW2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="LX2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="LY2" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>1.0633374392E10</v>
+        <v>1.0689954674E10</v>
       </c>
       <c r="B3">
-        <v>2.28637564E8</v>
+        <v>2.31929806E8</v>
       </c>
       <c r="C3" s="2">
-        <v>43556.49988425926</v>
+        <v>43581.38877314814</v>
       </c>
       <c r="D3" s="2">
-        <v>43557.88546296296</v>
+        <v>43581.43297453703</v>
       </c>
       <c r="E3" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="F3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="J3" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="K3" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="L3" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="M3" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="N3" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="O3" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="P3" t="s">
-        <v>297</v>
+        <v>300</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>301</v>
+      </c>
+      <c r="R3" t="s">
+        <v>302</v>
       </c>
       <c r="T3" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="U3">
-        <v>679.0</v>
+        <v>558.0</v>
       </c>
       <c r="V3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="W3">
-        <v>4.0</v>
+        <v>18.0</v>
       </c>
       <c r="X3">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="Y3" t="s">
-        <v>300</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>92</v>
+        <v>305</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>93</v>
       </c>
       <c r="AE3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AM3" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="AN3" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="AO3" t="s">
-        <v>303</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>304</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>305</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>306</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AT3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AU3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AV3" t="s">
         <v>310</v>
@@ -3337,361 +3460,271 @@
       <c r="BA3" t="s">
         <v>315</v>
       </c>
-      <c r="BB3">
-        <v>2.0</v>
-      </c>
-      <c r="BC3">
-        <v>4.0</v>
-      </c>
-      <c r="BD3">
-        <v>4.0</v>
-      </c>
-      <c r="BE3">
-        <v>40.0</v>
-      </c>
-      <c r="BF3">
-        <v>40.0</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>316</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>316</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>316</v>
-      </c>
       <c r="BJ3" t="s">
         <v>316</v>
       </c>
       <c r="BK3" t="s">
         <v>316</v>
       </c>
-      <c r="BL3" t="s">
+      <c r="BO3" t="s">
         <v>317</v>
       </c>
-      <c r="BM3" t="s">
+      <c r="BT3" t="s">
+        <v>314</v>
+      </c>
+      <c r="BU3" t="s">
         <v>318</v>
       </c>
-      <c r="BN3" t="s">
+      <c r="BZ3" t="s">
         <v>319</v>
       </c>
-      <c r="BQ3" t="s">
+      <c r="CA3" t="s">
         <v>320</v>
       </c>
-      <c r="BR3" t="s">
+      <c r="CB3" t="s">
         <v>321</v>
       </c>
-      <c r="BS3" t="s">
-        <v>321</v>
-      </c>
-      <c r="BT3" t="s">
+      <c r="CI3" t="s">
         <v>322</v>
       </c>
-      <c r="BU3" t="s">
-        <v>321</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>321</v>
-      </c>
-      <c r="BW3" t="s">
+      <c r="CM3" t="s">
         <v>323</v>
       </c>
-      <c r="BX3" t="s">
+      <c r="CN3" t="s">
         <v>324</v>
       </c>
-      <c r="BY3" t="s">
+      <c r="CP3" t="s">
         <v>325</v>
       </c>
-      <c r="BZ3" t="s">
+      <c r="CQ3" t="s">
         <v>326</v>
       </c>
-      <c r="CF3" t="s">
+      <c r="CS3" t="s">
         <v>327</v>
       </c>
-      <c r="CG3" t="s">
+      <c r="CT3" t="s">
         <v>328</v>
       </c>
-      <c r="CH3" t="s">
+      <c r="CV3" t="s">
         <v>329</v>
       </c>
-      <c r="CI3" t="s">
+      <c r="CW3" t="s">
         <v>330</v>
       </c>
-      <c r="CK3" t="s">
+      <c r="CX3" t="s">
         <v>331</v>
       </c>
-      <c r="CL3" t="s">
+      <c r="CY3" t="s">
         <v>332</v>
       </c>
-      <c r="CS3" t="s">
-        <v>291</v>
-      </c>
-      <c r="CT3" t="s">
+      <c r="DC3" t="s">
         <v>333</v>
-      </c>
-      <c r="CU3" t="s">
-        <v>334</v>
-      </c>
-      <c r="DD3" t="s">
-        <v>132</v>
-      </c>
-      <c r="DE3" t="s">
-        <v>133</v>
-      </c>
-      <c r="DF3" t="s">
-        <v>134</v>
-      </c>
-      <c r="DH3" t="s">
-        <v>136</v>
-      </c>
-      <c r="DO3" t="s">
-        <v>143</v>
-      </c>
-      <c r="FA3" t="s">
-        <v>99</v>
-      </c>
-      <c r="FI3" t="s">
-        <v>159</v>
-      </c>
-      <c r="GL3" t="s">
-        <v>99</v>
-      </c>
-      <c r="GU3" t="s">
-        <v>335</v>
-      </c>
-      <c r="IG3" t="s">
-        <v>225</v>
-      </c>
-      <c r="IV3" t="s">
-        <v>336</v>
-      </c>
-      <c r="KH3" t="s">
-        <v>270</v>
-      </c>
-      <c r="KU3" t="s">
-        <v>278</v>
-      </c>
-      <c r="KV3" t="s">
-        <v>279</v>
-      </c>
-      <c r="LE3" t="s">
-        <v>337</v>
-      </c>
-      <c r="LG3" t="s">
-        <v>338</v>
-      </c>
-      <c r="LH3" t="s">
-        <v>339</v>
-      </c>
-      <c r="LN3" t="s">
-        <v>340</v>
-      </c>
-      <c r="LO3" t="s">
-        <v>341</v>
-      </c>
-      <c r="LU3" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>1.0632772284E10</v>
+        <v>1.0633374392E10</v>
       </c>
       <c r="B4">
         <v>2.28637564E8</v>
       </c>
       <c r="C4" s="2">
-        <v>43556.35381944444</v>
+        <v>43556.49988425926</v>
       </c>
       <c r="D4" s="2">
-        <v>43557.57269675926</v>
+        <v>43557.88546296296</v>
       </c>
       <c r="E4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F4" t="s">
+        <v>335</v>
+      </c>
+      <c r="J4" t="s">
+        <v>335</v>
+      </c>
+      <c r="K4" t="s">
+        <v>336</v>
+      </c>
+      <c r="L4" t="s">
+        <v>337</v>
+      </c>
+      <c r="M4" t="s">
+        <v>338</v>
+      </c>
+      <c r="N4" t="s">
+        <v>339</v>
+      </c>
+      <c r="O4" t="s">
+        <v>340</v>
+      </c>
+      <c r="P4" t="s">
+        <v>341</v>
+      </c>
+      <c r="T4" t="s">
+        <v>342</v>
+      </c>
+      <c r="U4">
+        <v>679.0</v>
+      </c>
+      <c r="V4" t="s">
+        <v>304</v>
+      </c>
+      <c r="W4">
+        <v>4.0</v>
+      </c>
+      <c r="X4">
+        <v>0.0</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>305</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM4" t="s">
         <v>343</v>
       </c>
-      <c r="F4" t="s">
+      <c r="AN4" t="s">
         <v>344</v>
       </c>
-      <c r="J4" t="s">
-        <v>344</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="AO4" t="s">
         <v>345</v>
       </c>
-      <c r="L4" t="s">
-        <v>345</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="AP4" t="s">
         <v>346</v>
       </c>
-      <c r="N4" t="s">
+      <c r="AQ4" t="s">
         <v>347</v>
       </c>
-      <c r="O4" t="s">
+      <c r="AR4" t="s">
         <v>348</v>
       </c>
-      <c r="P4" t="s">
+      <c r="AS4" t="s">
         <v>349</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="AT4" t="s">
         <v>350</v>
       </c>
-      <c r="R4" t="s">
+      <c r="AU4" t="s">
+        <v>310</v>
+      </c>
+      <c r="AZ4" t="s">
         <v>351</v>
       </c>
-      <c r="T4" t="s">
+      <c r="BA4" t="s">
         <v>352</v>
       </c>
-      <c r="U4">
-        <v>607.0</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="BB4" t="s">
         <v>353</v>
       </c>
-      <c r="W4">
-        <v>21.0</v>
-      </c>
-      <c r="X4">
-        <v>3.0</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="BC4" t="s">
         <v>354</v>
       </c>
-      <c r="AB4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>100</v>
-      </c>
-      <c r="AN4" t="s">
+      <c r="BD4" t="s">
         <v>355</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="BE4">
+        <v>2.0</v>
+      </c>
+      <c r="BF4">
+        <v>4.0</v>
+      </c>
+      <c r="BG4">
+        <v>4.0</v>
+      </c>
+      <c r="BH4">
+        <v>40.0</v>
+      </c>
+      <c r="BI4">
+        <v>40.0</v>
+      </c>
+      <c r="BJ4" t="s">
         <v>356</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="BK4" t="s">
+        <v>356</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>356</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>356</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>356</v>
+      </c>
+      <c r="BO4" t="s">
         <v>357</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="BP4" t="s">
         <v>358</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="BQ4" t="s">
         <v>359</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="BT4" t="s">
         <v>360</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="BU4" t="s">
         <v>361</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="BV4" t="s">
+        <v>361</v>
+      </c>
+      <c r="BW4" t="s">
         <v>362</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="BX4" t="s">
+        <v>361</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>361</v>
+      </c>
+      <c r="BZ4" t="s">
         <v>363</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="CA4" t="s">
         <v>364</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="CB4" t="s">
         <v>365</v>
       </c>
-      <c r="BG4" t="s">
-        <v>316</v>
-      </c>
-      <c r="BL4" t="s">
+      <c r="CC4" t="s">
         <v>366</v>
       </c>
-      <c r="BQ4" t="s">
+      <c r="CI4" t="s">
+        <v>322</v>
+      </c>
+      <c r="CJ4" t="s">
         <v>367</v>
       </c>
-      <c r="BR4" t="s">
+      <c r="CK4" t="s">
         <v>368</v>
       </c>
-      <c r="BS4" t="s">
+      <c r="CL4" t="s">
         <v>369</v>
       </c>
-      <c r="BT4" t="s">
-        <v>369</v>
-      </c>
-      <c r="BU4" t="s">
-        <v>369</v>
-      </c>
-      <c r="BV4" t="s">
-        <v>369</v>
-      </c>
-      <c r="BW4" t="s">
+      <c r="CN4" t="s">
         <v>370</v>
       </c>
-      <c r="BY4" t="s">
-        <v>327</v>
-      </c>
-      <c r="CF4" t="s">
-        <v>327</v>
-      </c>
-      <c r="CG4" t="s">
+      <c r="CO4" t="s">
         <v>371</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="CV4" t="s">
+        <v>335</v>
+      </c>
+      <c r="CW4" t="s">
         <v>372</v>
       </c>
-      <c r="CI4" t="s">
+      <c r="CX4" t="s">
         <v>373</v>
       </c>
-      <c r="CJ4" t="s">
-        <v>374</v>
-      </c>
-      <c r="CK4" t="s">
-        <v>375</v>
-      </c>
-      <c r="CL4" t="s">
-        <v>376</v>
-      </c>
-      <c r="CM4" t="s">
-        <v>377</v>
-      </c>
-      <c r="CN4" t="s">
-        <v>378</v>
-      </c>
-      <c r="CO4" t="s">
-        <v>379</v>
-      </c>
-      <c r="CP4" t="s">
-        <v>380</v>
-      </c>
-      <c r="CQ4" t="s">
-        <v>381</v>
-      </c>
-      <c r="CR4" t="s">
-        <v>382</v>
-      </c>
-      <c r="CS4" t="s">
-        <v>383</v>
-      </c>
-      <c r="CT4" t="s">
-        <v>384</v>
-      </c>
-      <c r="CU4" t="s">
-        <v>385</v>
-      </c>
-      <c r="CV4" t="s">
-        <v>386</v>
-      </c>
-      <c r="CY4" t="s">
-        <v>371</v>
-      </c>
-      <c r="CZ4" t="s">
-        <v>387</v>
-      </c>
-      <c r="DA4" t="s">
-        <v>388</v>
-      </c>
-      <c r="DD4" t="s">
-        <v>132</v>
+      <c r="DG4" t="s">
+        <v>135</v>
       </c>
       <c r="DH4" t="s">
         <v>136</v>
@@ -3699,227 +3732,32 @@
       <c r="DI4" t="s">
         <v>137</v>
       </c>
-      <c r="DJ4" t="s">
-        <v>138</v>
-      </c>
       <c r="DK4" t="s">
         <v>139</v>
       </c>
-      <c r="DL4" t="s">
-        <v>140</v>
-      </c>
-      <c r="DM4" t="s">
-        <v>141</v>
-      </c>
-      <c r="DN4" t="s">
-        <v>142</v>
-      </c>
-      <c r="DO4" t="s">
-        <v>143</v>
-      </c>
-      <c r="DP4" t="s">
-        <v>144</v>
-      </c>
-      <c r="DQ4" t="s">
-        <v>145</v>
-      </c>
       <c r="DR4" t="s">
         <v>146</v>
       </c>
-      <c r="DV4" t="s">
-        <v>148</v>
-      </c>
-      <c r="DW4" t="s">
-        <v>149</v>
-      </c>
-      <c r="DX4" t="s">
-        <v>150</v>
-      </c>
-      <c r="DY4" t="s">
-        <v>151</v>
-      </c>
-      <c r="EA4" t="s">
-        <v>153</v>
-      </c>
-      <c r="EI4" t="s">
-        <v>161</v>
-      </c>
-      <c r="EP4" t="s">
-        <v>168</v>
-      </c>
-      <c r="FC4" t="s">
-        <v>179</v>
-      </c>
       <c r="FD4" t="s">
-        <v>180</v>
-      </c>
-      <c r="FE4" t="s">
-        <v>152</v>
-      </c>
-      <c r="FF4" t="s">
-        <v>154</v>
-      </c>
-      <c r="FG4" t="s">
-        <v>156</v>
-      </c>
-      <c r="FH4" t="s">
-        <v>157</v>
-      </c>
-      <c r="FI4" t="s">
-        <v>159</v>
-      </c>
-      <c r="FJ4" t="s">
-        <v>160</v>
-      </c>
-      <c r="FK4" t="s">
-        <v>161</v>
+        <v>102</v>
       </c>
       <c r="FL4" t="s">
         <v>162</v>
       </c>
-      <c r="FM4" t="s">
-        <v>163</v>
-      </c>
-      <c r="FN4" t="s">
-        <v>166</v>
-      </c>
-      <c r="FO4" t="s">
-        <v>169</v>
-      </c>
-      <c r="FP4" t="s">
-        <v>170</v>
-      </c>
-      <c r="FQ4" t="s">
-        <v>171</v>
-      </c>
-      <c r="FR4" t="s">
-        <v>172</v>
-      </c>
-      <c r="FS4" t="s">
-        <v>173</v>
-      </c>
-      <c r="FT4" t="s">
-        <v>174</v>
-      </c>
-      <c r="FU4" t="s">
-        <v>176</v>
-      </c>
-      <c r="FV4" t="s">
-        <v>177</v>
-      </c>
-      <c r="FZ4" t="s">
-        <v>182</v>
-      </c>
-      <c r="GA4" t="s">
-        <v>183</v>
-      </c>
-      <c r="GB4" t="s">
-        <v>184</v>
-      </c>
-      <c r="GC4" t="s">
-        <v>161</v>
-      </c>
-      <c r="GD4" t="s">
-        <v>163</v>
-      </c>
-      <c r="GE4" t="s">
-        <v>164</v>
-      </c>
-      <c r="GF4" t="s">
-        <v>165</v>
-      </c>
-      <c r="GG4" t="s">
-        <v>174</v>
-      </c>
-      <c r="GH4" t="s">
-        <v>185</v>
-      </c>
-      <c r="GI4" t="s">
-        <v>186</v>
-      </c>
-      <c r="GJ4" t="s">
-        <v>177</v>
-      </c>
-      <c r="GN4" t="s">
-        <v>188</v>
-      </c>
-      <c r="GU4" t="s">
-        <v>389</v>
-      </c>
-      <c r="IK4" t="s">
+      <c r="GO4" t="s">
+        <v>102</v>
+      </c>
+      <c r="GX4" t="s">
+        <v>374</v>
+      </c>
+      <c r="IJ4" t="s">
         <v>228</v>
       </c>
-      <c r="IM4" t="s">
-        <v>230</v>
-      </c>
-      <c r="IN4" t="s">
-        <v>231</v>
-      </c>
-      <c r="IO4" t="s">
-        <v>232</v>
-      </c>
-      <c r="IP4" t="s">
-        <v>170</v>
-      </c>
-      <c r="IQ4" t="s">
-        <v>233</v>
-      </c>
-      <c r="IR4" t="s">
-        <v>234</v>
-      </c>
-      <c r="IS4" t="s">
-        <v>235</v>
-      </c>
-      <c r="IW4" t="s">
-        <v>237</v>
-      </c>
-      <c r="IZ4" t="s">
-        <v>240</v>
-      </c>
-      <c r="JC4" t="s">
-        <v>243</v>
-      </c>
-      <c r="JG4" t="s">
-        <v>247</v>
-      </c>
-      <c r="JH4" t="s">
-        <v>248</v>
-      </c>
-      <c r="JI4" t="s">
-        <v>249</v>
-      </c>
-      <c r="JZ4" t="s">
-        <v>264</v>
-      </c>
-      <c r="KB4" t="s">
-        <v>266</v>
-      </c>
-      <c r="KD4" t="s">
-        <v>268</v>
-      </c>
-      <c r="KG4" t="s">
-        <v>269</v>
-      </c>
-      <c r="KH4" t="s">
-        <v>270</v>
-      </c>
-      <c r="KI4" t="s">
-        <v>231</v>
-      </c>
-      <c r="KJ4" t="s">
-        <v>271</v>
-      </c>
-      <c r="KQ4" t="s">
-        <v>276</v>
-      </c>
-      <c r="KU4" t="s">
-        <v>278</v>
-      </c>
-      <c r="KV4" t="s">
-        <v>279</v>
-      </c>
-      <c r="KW4" t="s">
-        <v>280</v>
+      <c r="IY4" t="s">
+        <v>375</v>
+      </c>
+      <c r="KK4" t="s">
+        <v>273</v>
       </c>
       <c r="KX4" t="s">
         <v>281</v>
@@ -3927,680 +3765,920 @@
       <c r="KY4" t="s">
         <v>282</v>
       </c>
-      <c r="KZ4" t="s">
-        <v>283</v>
-      </c>
-      <c r="LA4" t="s">
-        <v>284</v>
-      </c>
-      <c r="LB4" t="s">
-        <v>285</v>
-      </c>
-      <c r="LF4" t="s">
-        <v>390</v>
-      </c>
-      <c r="LG4" t="s">
-        <v>391</v>
-      </c>
       <c r="LH4" t="s">
-        <v>392</v>
-      </c>
-      <c r="LI4" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="LJ4" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
       <c r="LK4" t="s">
-        <v>395</v>
-      </c>
-      <c r="LM4" t="s">
-        <v>396</v>
-      </c>
-      <c r="LN4" t="s">
-        <v>397</v>
-      </c>
-      <c r="LP4" t="s">
-        <v>398</v>
-      </c>
-      <c r="LU4" t="s">
-        <v>399</v>
+        <v>378</v>
+      </c>
+      <c r="LQ4" t="s">
+        <v>379</v>
+      </c>
+      <c r="LR4" t="s">
+        <v>380</v>
+      </c>
+      <c r="LX4" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>1.0626043328E10</v>
+        <v>1.0632772284E10</v>
       </c>
       <c r="B5">
         <v>2.28637564E8</v>
       </c>
       <c r="C5" s="2">
-        <v>43552.51997685185</v>
+        <v>43556.35381944444</v>
       </c>
       <c r="D5" s="2">
-        <v>43557.43107638889</v>
+        <v>43557.57269675926</v>
       </c>
       <c r="E5" t="s">
+        <v>382</v>
+      </c>
+      <c r="F5" t="s">
+        <v>383</v>
+      </c>
+      <c r="J5" t="s">
+        <v>383</v>
+      </c>
+      <c r="K5" t="s">
+        <v>384</v>
+      </c>
+      <c r="L5" t="s">
+        <v>384</v>
+      </c>
+      <c r="M5" t="s">
+        <v>385</v>
+      </c>
+      <c r="N5" t="s">
+        <v>386</v>
+      </c>
+      <c r="O5" t="s">
+        <v>387</v>
+      </c>
+      <c r="P5" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>389</v>
+      </c>
+      <c r="R5" t="s">
+        <v>390</v>
+      </c>
+      <c r="T5" t="s">
+        <v>391</v>
+      </c>
+      <c r="U5">
+        <v>607.0</v>
+      </c>
+      <c r="V5" t="s">
+        <v>392</v>
+      </c>
+      <c r="W5">
+        <v>21.0</v>
+      </c>
+      <c r="X5">
+        <v>3.0</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>393</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>394</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>395</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>396</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>397</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>398</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>399</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>309</v>
+      </c>
+      <c r="AU5" t="s">
         <v>400</v>
       </c>
-      <c r="F5" t="s">
+      <c r="AZ5" t="s">
         <v>401</v>
       </c>
-      <c r="J5" t="s">
+      <c r="BE5" t="s">
         <v>402</v>
       </c>
-      <c r="K5" t="s">
+      <c r="BJ5" t="s">
+        <v>356</v>
+      </c>
+      <c r="BO5" t="s">
         <v>403</v>
       </c>
-      <c r="L5" t="s">
+      <c r="BT5" t="s">
         <v>404</v>
       </c>
-      <c r="M5" t="s">
+      <c r="BU5" t="s">
         <v>405</v>
       </c>
-      <c r="N5" t="s">
+      <c r="BV5" t="s">
         <v>406</v>
       </c>
-      <c r="O5" t="s">
+      <c r="BW5" t="s">
+        <v>406</v>
+      </c>
+      <c r="BX5" t="s">
+        <v>406</v>
+      </c>
+      <c r="BY5" t="s">
+        <v>406</v>
+      </c>
+      <c r="BZ5" t="s">
         <v>407</v>
       </c>
-      <c r="P5" t="s">
+      <c r="CB5" t="s">
+        <v>322</v>
+      </c>
+      <c r="CI5" t="s">
+        <v>322</v>
+      </c>
+      <c r="CJ5" t="s">
         <v>408</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="CK5" t="s">
         <v>409</v>
       </c>
-      <c r="R5" t="s">
+      <c r="CL5" t="s">
         <v>410</v>
       </c>
-      <c r="T5" t="s">
+      <c r="CM5" t="s">
         <v>411</v>
       </c>
-      <c r="U5" t="s">
+      <c r="CN5" t="s">
         <v>412</v>
       </c>
-      <c r="V5" t="s">
-        <v>299</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="CO5" t="s">
         <v>413</v>
       </c>
-      <c r="X5" t="s">
+      <c r="CP5" t="s">
         <v>414</v>
       </c>
-      <c r="Y5" t="s">
-        <v>354</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>89</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>355</v>
-      </c>
-      <c r="AO5" t="s">
+      <c r="CQ5" t="s">
         <v>415</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="CR5" t="s">
         <v>416</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="CS5" t="s">
         <v>417</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="CT5" t="s">
         <v>418</v>
       </c>
-      <c r="AU5" t="s">
-        <v>309</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>310</v>
-      </c>
-      <c r="AW5" t="s">
+      <c r="CU5" t="s">
         <v>419</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="CV5" t="s">
         <v>420</v>
       </c>
-      <c r="AY5" t="s">
+      <c r="CW5" t="s">
         <v>421</v>
       </c>
-      <c r="BB5">
-        <v>40.0</v>
-      </c>
-      <c r="BC5">
-        <v>5.0</v>
-      </c>
-      <c r="BD5" t="s">
+      <c r="CX5" t="s">
         <v>422</v>
       </c>
-      <c r="BG5" t="s">
-        <v>316</v>
-      </c>
-      <c r="BH5" t="s">
-        <v>316</v>
-      </c>
-      <c r="BI5" t="s">
-        <v>316</v>
-      </c>
-      <c r="BL5" t="s">
+      <c r="CY5" t="s">
         <v>423</v>
       </c>
-      <c r="BM5" t="s">
+      <c r="DB5" t="s">
+        <v>408</v>
+      </c>
+      <c r="DC5" t="s">
         <v>424</v>
       </c>
-      <c r="BQ5" t="s">
+      <c r="DD5" t="s">
         <v>425</v>
       </c>
-      <c r="BR5" t="s">
-        <v>426</v>
-      </c>
-      <c r="BS5" t="s">
-        <v>427</v>
-      </c>
-      <c r="BW5" t="s">
-        <v>428</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>429</v>
-      </c>
-      <c r="BY5" t="s">
-        <v>430</v>
-      </c>
-      <c r="CF5" t="s">
-        <v>327</v>
-      </c>
-      <c r="CG5" t="s">
-        <v>431</v>
-      </c>
-      <c r="CH5" t="s">
-        <v>432</v>
-      </c>
-      <c r="CI5" t="s">
-        <v>433</v>
-      </c>
-      <c r="CS5" t="s">
-        <v>402</v>
-      </c>
-      <c r="CT5" t="s">
-        <v>434</v>
-      </c>
-      <c r="CU5" t="s">
-        <v>435</v>
-      </c>
-      <c r="CV5" t="s">
-        <v>436</v>
-      </c>
-      <c r="CW5" t="s">
-        <v>409</v>
-      </c>
-      <c r="CX5" t="s">
-        <v>437</v>
-      </c>
-      <c r="DD5" t="s">
-        <v>132</v>
-      </c>
-      <c r="DE5" t="s">
-        <v>133</v>
-      </c>
-      <c r="DF5" t="s">
-        <v>134</v>
+      <c r="DG5" t="s">
+        <v>135</v>
       </c>
       <c r="DK5" t="s">
         <v>139</v>
       </c>
+      <c r="DL5" t="s">
+        <v>140</v>
+      </c>
+      <c r="DM5" t="s">
+        <v>141</v>
+      </c>
+      <c r="DN5" t="s">
+        <v>142</v>
+      </c>
       <c r="DO5" t="s">
         <v>143</v>
       </c>
-      <c r="DW5" t="s">
+      <c r="DP5" t="s">
+        <v>144</v>
+      </c>
+      <c r="DQ5" t="s">
+        <v>145</v>
+      </c>
+      <c r="DR5" t="s">
+        <v>146</v>
+      </c>
+      <c r="DS5" t="s">
+        <v>147</v>
+      </c>
+      <c r="DT5" t="s">
+        <v>148</v>
+      </c>
+      <c r="DU5" t="s">
         <v>149</v>
       </c>
-      <c r="EP5" t="s">
+      <c r="DY5" t="s">
+        <v>151</v>
+      </c>
+      <c r="DZ5" t="s">
+        <v>152</v>
+      </c>
+      <c r="EA5" t="s">
+        <v>153</v>
+      </c>
+      <c r="EB5" t="s">
+        <v>154</v>
+      </c>
+      <c r="ED5" t="s">
+        <v>156</v>
+      </c>
+      <c r="EL5" t="s">
+        <v>164</v>
+      </c>
+      <c r="ES5" t="s">
+        <v>171</v>
+      </c>
+      <c r="FF5" t="s">
+        <v>182</v>
+      </c>
+      <c r="FG5" t="s">
+        <v>183</v>
+      </c>
+      <c r="FH5" t="s">
+        <v>155</v>
+      </c>
+      <c r="FI5" t="s">
+        <v>157</v>
+      </c>
+      <c r="FJ5" t="s">
+        <v>159</v>
+      </c>
+      <c r="FK5" t="s">
+        <v>160</v>
+      </c>
+      <c r="FL5" t="s">
+        <v>162</v>
+      </c>
+      <c r="FM5" t="s">
+        <v>163</v>
+      </c>
+      <c r="FN5" t="s">
+        <v>164</v>
+      </c>
+      <c r="FO5" t="s">
+        <v>165</v>
+      </c>
+      <c r="FP5" t="s">
+        <v>166</v>
+      </c>
+      <c r="FQ5" t="s">
+        <v>169</v>
+      </c>
+      <c r="FR5" t="s">
+        <v>172</v>
+      </c>
+      <c r="FS5" t="s">
+        <v>173</v>
+      </c>
+      <c r="FT5" t="s">
+        <v>174</v>
+      </c>
+      <c r="FU5" t="s">
+        <v>175</v>
+      </c>
+      <c r="FV5" t="s">
+        <v>176</v>
+      </c>
+      <c r="FW5" t="s">
+        <v>177</v>
+      </c>
+      <c r="FX5" t="s">
+        <v>179</v>
+      </c>
+      <c r="FY5" t="s">
+        <v>180</v>
+      </c>
+      <c r="GC5" t="s">
+        <v>185</v>
+      </c>
+      <c r="GD5" t="s">
+        <v>186</v>
+      </c>
+      <c r="GE5" t="s">
+        <v>187</v>
+      </c>
+      <c r="GF5" t="s">
+        <v>164</v>
+      </c>
+      <c r="GG5" t="s">
+        <v>166</v>
+      </c>
+      <c r="GH5" t="s">
+        <v>167</v>
+      </c>
+      <c r="GI5" t="s">
         <v>168</v>
       </c>
-      <c r="FD5" t="s">
+      <c r="GJ5" t="s">
+        <v>177</v>
+      </c>
+      <c r="GK5" t="s">
+        <v>188</v>
+      </c>
+      <c r="GL5" t="s">
+        <v>189</v>
+      </c>
+      <c r="GM5" t="s">
         <v>180</v>
       </c>
-      <c r="FQ5" t="s">
-        <v>171</v>
-      </c>
-      <c r="GA5" t="s">
-        <v>183</v>
-      </c>
-      <c r="GS5" t="s">
-        <v>99</v>
-      </c>
-      <c r="GV5" t="s">
-        <v>438</v>
-      </c>
-      <c r="GW5" t="s">
-        <v>439</v>
+      <c r="GQ5" t="s">
+        <v>191</v>
       </c>
       <c r="GX5" t="s">
-        <v>440</v>
-      </c>
-      <c r="GY5" t="s">
-        <v>441</v>
-      </c>
-      <c r="GZ5" t="s">
-        <v>442</v>
-      </c>
-      <c r="HI5" t="s">
-        <v>202</v>
-      </c>
-      <c r="HJ5" t="s">
-        <v>203</v>
-      </c>
-      <c r="HK5" t="s">
-        <v>204</v>
-      </c>
-      <c r="HL5" t="s">
-        <v>205</v>
-      </c>
-      <c r="IO5" t="s">
-        <v>232</v>
+        <v>426</v>
+      </c>
+      <c r="IN5" t="s">
+        <v>231</v>
+      </c>
+      <c r="IP5" t="s">
+        <v>233</v>
       </c>
       <c r="IQ5" t="s">
-        <v>233</v>
-      </c>
-      <c r="IW5" t="s">
+        <v>234</v>
+      </c>
+      <c r="IR5" t="s">
+        <v>235</v>
+      </c>
+      <c r="IS5" t="s">
+        <v>173</v>
+      </c>
+      <c r="IT5" t="s">
+        <v>236</v>
+      </c>
+      <c r="IU5" t="s">
         <v>237</v>
       </c>
-      <c r="IX5" t="s">
+      <c r="IV5" t="s">
         <v>238</v>
       </c>
-      <c r="IY5" t="s">
-        <v>239</v>
-      </c>
-      <c r="JH5" t="s">
-        <v>248</v>
-      </c>
-      <c r="KB5" t="s">
-        <v>266</v>
-      </c>
-      <c r="KU5" t="s">
-        <v>278</v>
-      </c>
-      <c r="KV5" t="s">
+      <c r="IZ5" t="s">
+        <v>240</v>
+      </c>
+      <c r="JC5" t="s">
+        <v>243</v>
+      </c>
+      <c r="JF5" t="s">
+        <v>246</v>
+      </c>
+      <c r="JJ5" t="s">
+        <v>250</v>
+      </c>
+      <c r="JK5" t="s">
+        <v>251</v>
+      </c>
+      <c r="JL5" t="s">
+        <v>252</v>
+      </c>
+      <c r="KC5" t="s">
+        <v>267</v>
+      </c>
+      <c r="KE5" t="s">
+        <v>269</v>
+      </c>
+      <c r="KG5" t="s">
+        <v>271</v>
+      </c>
+      <c r="KJ5" t="s">
+        <v>272</v>
+      </c>
+      <c r="KK5" t="s">
+        <v>273</v>
+      </c>
+      <c r="KL5" t="s">
+        <v>234</v>
+      </c>
+      <c r="KM5" t="s">
+        <v>274</v>
+      </c>
+      <c r="KT5" t="s">
         <v>279</v>
-      </c>
-      <c r="KW5" t="s">
-        <v>280</v>
       </c>
       <c r="KX5" t="s">
         <v>281</v>
       </c>
+      <c r="KY5" t="s">
+        <v>282</v>
+      </c>
+      <c r="KZ5" t="s">
+        <v>283</v>
+      </c>
+      <c r="LA5" t="s">
+        <v>284</v>
+      </c>
+      <c r="LB5" t="s">
+        <v>285</v>
+      </c>
+      <c r="LC5" t="s">
+        <v>286</v>
+      </c>
+      <c r="LD5" t="s">
+        <v>287</v>
+      </c>
       <c r="LE5" t="s">
-        <v>443</v>
-      </c>
-      <c r="LG5" t="s">
-        <v>444</v>
+        <v>288</v>
+      </c>
+      <c r="LI5" t="s">
+        <v>427</v>
+      </c>
+      <c r="LJ5" t="s">
+        <v>428</v>
+      </c>
+      <c r="LK5" t="s">
+        <v>429</v>
+      </c>
+      <c r="LL5" t="s">
+        <v>430</v>
       </c>
       <c r="LM5" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
       <c r="LN5" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="LP5" t="s">
-        <v>447</v>
-      </c>
-      <c r="LV5" t="s">
-        <v>448</v>
+        <v>433</v>
+      </c>
+      <c r="LQ5" t="s">
+        <v>434</v>
+      </c>
+      <c r="LS5" t="s">
+        <v>435</v>
+      </c>
+      <c r="LX5" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>1.0551569639E10</v>
+        <v>1.0626043328E10</v>
       </c>
       <c r="B6">
-        <v>2.26101601E8</v>
+        <v>2.28637564E8</v>
       </c>
       <c r="C6" s="2">
-        <v>43520.39091435185</v>
+        <v>43552.51997685185</v>
       </c>
       <c r="D6" s="2">
-        <v>43532.62158564815</v>
+        <v>43557.43107638889</v>
       </c>
       <c r="E6" t="s">
+        <v>437</v>
+      </c>
+      <c r="F6" t="s">
+        <v>438</v>
+      </c>
+      <c r="J6" t="s">
+        <v>439</v>
+      </c>
+      <c r="K6" t="s">
+        <v>440</v>
+      </c>
+      <c r="L6" t="s">
+        <v>441</v>
+      </c>
+      <c r="M6" t="s">
+        <v>442</v>
+      </c>
+      <c r="N6" t="s">
+        <v>443</v>
+      </c>
+      <c r="O6" t="s">
+        <v>444</v>
+      </c>
+      <c r="P6" t="s">
+        <v>445</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>446</v>
+      </c>
+      <c r="R6" t="s">
+        <v>447</v>
+      </c>
+      <c r="T6" t="s">
+        <v>448</v>
+      </c>
+      <c r="U6" t="s">
         <v>449</v>
       </c>
-      <c r="J6" t="s">
+      <c r="V6" t="s">
+        <v>304</v>
+      </c>
+      <c r="W6" t="s">
         <v>450</v>
       </c>
-      <c r="K6" t="s">
+      <c r="X6" t="s">
         <v>451</v>
       </c>
-      <c r="L6" t="s">
+      <c r="Y6" t="s">
+        <v>393</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN6" t="s">
         <v>452</v>
       </c>
-      <c r="M6" t="s">
+      <c r="AO6" t="s">
         <v>453</v>
       </c>
-      <c r="N6" t="s">
+      <c r="AP6" t="s">
         <v>454</v>
       </c>
-      <c r="O6" t="s">
+      <c r="AQ6" t="s">
         <v>455</v>
       </c>
-      <c r="P6" t="s">
+      <c r="AT6" t="s">
+        <v>350</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>310</v>
+      </c>
+      <c r="AZ6" t="s">
         <v>456</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="BA6" t="s">
         <v>457</v>
       </c>
-      <c r="R6" t="s">
+      <c r="BB6" t="s">
         <v>458</v>
       </c>
-      <c r="T6" t="s">
+      <c r="BE6">
+        <v>40.0</v>
+      </c>
+      <c r="BF6">
+        <v>5.0</v>
+      </c>
+      <c r="BG6" t="s">
         <v>459</v>
       </c>
-      <c r="U6" t="s">
+      <c r="BJ6" t="s">
+        <v>356</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>356</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>356</v>
+      </c>
+      <c r="BO6" t="s">
         <v>460</v>
       </c>
-      <c r="V6" t="s">
-        <v>353</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>300</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>302</v>
-      </c>
-      <c r="AO6" t="s">
+      <c r="BP6" t="s">
         <v>461</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="BT6" t="s">
         <v>462</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="BU6" t="s">
         <v>463</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="BV6" t="s">
         <v>464</v>
       </c>
-      <c r="AU6" t="s">
-        <v>362</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>310</v>
-      </c>
-      <c r="AW6" t="s">
+      <c r="BZ6" t="s">
         <v>465</v>
       </c>
-      <c r="AX6" t="s">
-        <v>284</v>
-      </c>
-      <c r="BB6">
-        <v>2.0</v>
-      </c>
-      <c r="BC6">
-        <v>5.0</v>
-      </c>
-      <c r="BG6">
-        <v>16.0</v>
-      </c>
-      <c r="BH6">
-        <v>52.0</v>
-      </c>
-      <c r="BL6" t="s">
+      <c r="CA6" t="s">
         <v>466</v>
       </c>
-      <c r="BM6" t="s">
+      <c r="CB6" t="s">
         <v>467</v>
       </c>
-      <c r="BQ6" t="s">
+      <c r="CI6" t="s">
+        <v>322</v>
+      </c>
+      <c r="CJ6" t="s">
         <v>468</v>
       </c>
-      <c r="BR6" t="s">
+      <c r="CK6" t="s">
         <v>469</v>
       </c>
-      <c r="BS6" t="s">
+      <c r="CL6" t="s">
         <v>470</v>
       </c>
-      <c r="BZ6" t="s">
+      <c r="CV6" t="s">
+        <v>439</v>
+      </c>
+      <c r="CW6" t="s">
         <v>471</v>
       </c>
-      <c r="CC6" t="s">
-        <v>471</v>
-      </c>
-      <c r="CF6" t="s">
-        <v>327</v>
-      </c>
-      <c r="CH6" t="s">
+      <c r="CX6" t="s">
         <v>472</v>
       </c>
-      <c r="CI6" t="s">
+      <c r="CY6" t="s">
         <v>473</v>
       </c>
-      <c r="CK6" t="s">
+      <c r="CZ6" t="s">
+        <v>446</v>
+      </c>
+      <c r="DA6" t="s">
         <v>474</v>
       </c>
-      <c r="CL6" t="s">
-        <v>475</v>
-      </c>
-      <c r="CS6" t="s">
-        <v>476</v>
-      </c>
-      <c r="CT6" t="s">
-        <v>455</v>
-      </c>
-      <c r="CV6" t="s">
-        <v>456</v>
-      </c>
-      <c r="CW6" t="s">
-        <v>457</v>
-      </c>
-      <c r="CX6" t="s">
-        <v>458</v>
-      </c>
-      <c r="DK6" t="s">
-        <v>139</v>
-      </c>
-      <c r="DL6" t="s">
-        <v>140</v>
-      </c>
-      <c r="DM6" t="s">
-        <v>141</v>
-      </c>
-      <c r="DO6" t="s">
-        <v>143</v>
-      </c>
-      <c r="DP6" t="s">
-        <v>144</v>
-      </c>
-      <c r="DQ6" t="s">
-        <v>145</v>
+      <c r="DG6" t="s">
+        <v>135</v>
+      </c>
+      <c r="DH6" t="s">
+        <v>136</v>
+      </c>
+      <c r="DI6" t="s">
+        <v>137</v>
+      </c>
+      <c r="DN6" t="s">
+        <v>142</v>
       </c>
       <c r="DR6" t="s">
         <v>146</v>
       </c>
-      <c r="EX6" t="s">
-        <v>176</v>
-      </c>
-      <c r="FB6" t="s">
+      <c r="DZ6" t="s">
+        <v>152</v>
+      </c>
+      <c r="ES6" t="s">
+        <v>171</v>
+      </c>
+      <c r="FG6" t="s">
+        <v>183</v>
+      </c>
+      <c r="FT6" t="s">
+        <v>174</v>
+      </c>
+      <c r="GD6" t="s">
+        <v>186</v>
+      </c>
+      <c r="GV6" t="s">
+        <v>102</v>
+      </c>
+      <c r="GY6" t="s">
+        <v>475</v>
+      </c>
+      <c r="GZ6" t="s">
+        <v>476</v>
+      </c>
+      <c r="HA6" t="s">
         <v>477</v>
       </c>
-      <c r="GS6" t="s">
-        <v>99</v>
+      <c r="HB6" t="s">
+        <v>478</v>
+      </c>
+      <c r="HC6" t="s">
+        <v>479</v>
+      </c>
+      <c r="HL6" t="s">
+        <v>205</v>
+      </c>
+      <c r="HM6" t="s">
+        <v>206</v>
+      </c>
+      <c r="HN6" t="s">
+        <v>207</v>
+      </c>
+      <c r="HO6" t="s">
+        <v>208</v>
+      </c>
+      <c r="IR6" t="s">
+        <v>235</v>
       </c>
       <c r="IT6" t="s">
-        <v>99</v>
-      </c>
-      <c r="JH6" t="s">
-        <v>248</v>
-      </c>
-      <c r="JI6" t="s">
-        <v>249</v>
-      </c>
-      <c r="KU6" t="s">
-        <v>278</v>
-      </c>
-      <c r="KV6" t="s">
-        <v>279</v>
-      </c>
-      <c r="KW6" t="s">
-        <v>280</v>
+        <v>236</v>
+      </c>
+      <c r="IZ6" t="s">
+        <v>240</v>
+      </c>
+      <c r="JA6" t="s">
+        <v>241</v>
+      </c>
+      <c r="JB6" t="s">
+        <v>242</v>
+      </c>
+      <c r="JK6" t="s">
+        <v>251</v>
+      </c>
+      <c r="KE6" t="s">
+        <v>269</v>
       </c>
       <c r="KX6" t="s">
         <v>281</v>
       </c>
+      <c r="KY6" t="s">
+        <v>282</v>
+      </c>
       <c r="KZ6" t="s">
         <v>283</v>
       </c>
       <c r="LA6" t="s">
         <v>284</v>
       </c>
-      <c r="LF6" t="s">
-        <v>478</v>
-      </c>
-      <c r="LV6" t="s">
-        <v>479</v>
+      <c r="LH6" t="s">
+        <v>480</v>
+      </c>
+      <c r="LJ6" t="s">
+        <v>481</v>
+      </c>
+      <c r="LP6" t="s">
+        <v>482</v>
+      </c>
+      <c r="LQ6" t="s">
+        <v>483</v>
+      </c>
+      <c r="LS6" t="s">
+        <v>484</v>
+      </c>
+      <c r="LY6" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>1.0549086762E10</v>
+        <v>1.0551569639E10</v>
       </c>
       <c r="B7">
-        <v>2.26208327E8</v>
+        <v>2.26101601E8</v>
       </c>
       <c r="C7" s="2">
-        <v>43518.48881944444</v>
+        <v>43520.39091435185</v>
       </c>
       <c r="D7" s="2">
-        <v>43549.44997685185</v>
+        <v>43532.62158564815</v>
       </c>
       <c r="E7" t="s">
-        <v>480</v>
-      </c>
-      <c r="F7" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="J7" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="K7" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="L7" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="M7" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="N7" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="O7" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="P7" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="Q7" t="s">
-        <v>489</v>
+        <v>494</v>
+      </c>
+      <c r="R7" t="s">
+        <v>495</v>
       </c>
       <c r="T7" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="U7" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="V7" t="s">
-        <v>299</v>
+        <v>392</v>
       </c>
       <c r="Y7" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="AB7" t="s">
-        <v>90</v>
-      </c>
-      <c r="AM7" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>498</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>499</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>500</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>501</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>309</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>310</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>502</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>287</v>
+      </c>
+      <c r="BE7">
+        <v>2.0</v>
+      </c>
+      <c r="BF7">
+        <v>5.0</v>
+      </c>
+      <c r="BJ7">
+        <v>16.0</v>
+      </c>
+      <c r="BK7">
+        <v>52.0</v>
+      </c>
+      <c r="BO7" t="s">
+        <v>503</v>
+      </c>
+      <c r="BP7" t="s">
+        <v>504</v>
+      </c>
+      <c r="BT7" t="s">
+        <v>505</v>
+      </c>
+      <c r="BU7" t="s">
+        <v>506</v>
+      </c>
+      <c r="BV7" t="s">
+        <v>507</v>
+      </c>
+      <c r="CC7" t="s">
+        <v>508</v>
+      </c>
+      <c r="CF7" t="s">
+        <v>508</v>
+      </c>
+      <c r="CI7" t="s">
+        <v>322</v>
+      </c>
+      <c r="CK7" t="s">
+        <v>509</v>
+      </c>
+      <c r="CL7" t="s">
+        <v>510</v>
+      </c>
+      <c r="CN7" t="s">
+        <v>511</v>
+      </c>
+      <c r="CO7" t="s">
+        <v>512</v>
+      </c>
+      <c r="CV7" t="s">
+        <v>513</v>
+      </c>
+      <c r="CW7" t="s">
         <v>492</v>
       </c>
-      <c r="AN7" t="s">
-        <v>302</v>
-      </c>
-      <c r="AO7" t="s">
+      <c r="CY7" t="s">
         <v>493</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="CZ7" t="s">
         <v>494</v>
       </c>
-      <c r="AU7" t="s">
+      <c r="DA7" t="s">
         <v>495</v>
       </c>
-      <c r="AV7" t="s">
-        <v>496</v>
-      </c>
-      <c r="BQ7" t="s">
-        <v>497</v>
-      </c>
-      <c r="BR7" t="s">
-        <v>498</v>
-      </c>
-      <c r="BS7" t="s">
-        <v>499</v>
-      </c>
-      <c r="BT7" t="s">
-        <v>500</v>
-      </c>
-      <c r="BU7" t="s">
-        <v>501</v>
-      </c>
-      <c r="BZ7" t="s">
-        <v>502</v>
-      </c>
-      <c r="CA7" t="s">
-        <v>503</v>
-      </c>
-      <c r="CC7" t="s">
-        <v>504</v>
-      </c>
-      <c r="CD7" t="s">
-        <v>505</v>
-      </c>
-      <c r="CF7" t="s">
-        <v>327</v>
-      </c>
-      <c r="CG7" t="s">
-        <v>506</v>
-      </c>
-      <c r="CI7" t="s">
-        <v>507</v>
-      </c>
-      <c r="CS7" t="s">
-        <v>508</v>
-      </c>
-      <c r="CT7" t="s">
-        <v>509</v>
-      </c>
-      <c r="CU7" t="s">
-        <v>510</v>
-      </c>
-      <c r="CV7" t="s">
-        <v>511</v>
-      </c>
-      <c r="CW7" t="s">
-        <v>512</v>
-      </c>
-      <c r="CY7" t="s">
-        <v>513</v>
-      </c>
-      <c r="CZ7" t="s">
-        <v>514</v>
-      </c>
-      <c r="DA7" t="s">
-        <v>515</v>
-      </c>
-      <c r="DB7" t="s">
-        <v>516</v>
-      </c>
-      <c r="DK7" t="s">
-        <v>139</v>
+      <c r="DN7" t="s">
+        <v>142</v>
       </c>
       <c r="DO7" t="s">
         <v>143</v>
@@ -4608,156 +4686,357 @@
       <c r="DP7" t="s">
         <v>144</v>
       </c>
-      <c r="ES7" t="s">
-        <v>171</v>
-      </c>
-      <c r="FB7" t="s">
-        <v>517</v>
-      </c>
-      <c r="GS7" t="s">
-        <v>99</v>
-      </c>
-      <c r="IQ7" t="s">
-        <v>233</v>
-      </c>
-      <c r="KV7" t="s">
-        <v>279</v>
-      </c>
-      <c r="LE7" t="s">
-        <v>518</v>
-      </c>
-      <c r="LF7" t="s">
-        <v>519</v>
-      </c>
-      <c r="LK7" t="s">
-        <v>520</v>
-      </c>
-      <c r="LL7" t="s">
-        <v>521</v>
-      </c>
-      <c r="LM7" t="s">
-        <v>522</v>
+      <c r="DR7" t="s">
+        <v>146</v>
+      </c>
+      <c r="DS7" t="s">
+        <v>147</v>
+      </c>
+      <c r="DT7" t="s">
+        <v>148</v>
+      </c>
+      <c r="DU7" t="s">
+        <v>149</v>
+      </c>
+      <c r="FA7" t="s">
+        <v>179</v>
+      </c>
+      <c r="FE7" t="s">
+        <v>514</v>
+      </c>
+      <c r="GV7" t="s">
+        <v>102</v>
+      </c>
+      <c r="IW7" t="s">
+        <v>102</v>
+      </c>
+      <c r="JK7" t="s">
+        <v>251</v>
+      </c>
+      <c r="JL7" t="s">
+        <v>252</v>
+      </c>
+      <c r="KX7" t="s">
+        <v>281</v>
+      </c>
+      <c r="KY7" t="s">
+        <v>282</v>
+      </c>
+      <c r="KZ7" t="s">
+        <v>283</v>
+      </c>
+      <c r="LA7" t="s">
+        <v>284</v>
+      </c>
+      <c r="LC7" t="s">
+        <v>286</v>
+      </c>
+      <c r="LD7" t="s">
+        <v>287</v>
+      </c>
+      <c r="LI7" t="s">
+        <v>515</v>
+      </c>
+      <c r="LY7" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>1.0548992723E10</v>
+        <v>1.0549086762E10</v>
       </c>
       <c r="B8">
         <v>2.26208327E8</v>
       </c>
       <c r="C8" s="2">
+        <v>43518.48881944444</v>
+      </c>
+      <c r="D8" s="2">
+        <v>43549.44997685185</v>
+      </c>
+      <c r="E8" t="s">
+        <v>517</v>
+      </c>
+      <c r="F8" t="s">
+        <v>518</v>
+      </c>
+      <c r="J8" t="s">
+        <v>519</v>
+      </c>
+      <c r="K8" t="s">
+        <v>520</v>
+      </c>
+      <c r="L8" t="s">
+        <v>521</v>
+      </c>
+      <c r="M8" t="s">
+        <v>522</v>
+      </c>
+      <c r="N8" t="s">
+        <v>523</v>
+      </c>
+      <c r="O8" t="s">
+        <v>524</v>
+      </c>
+      <c r="P8" t="s">
+        <v>525</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>526</v>
+      </c>
+      <c r="T8" t="s">
+        <v>527</v>
+      </c>
+      <c r="U8" t="s">
+        <v>528</v>
+      </c>
+      <c r="V8" t="s">
+        <v>304</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>529</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>530</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>531</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>532</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>533</v>
+      </c>
+      <c r="BT8" t="s">
+        <v>534</v>
+      </c>
+      <c r="BU8" t="s">
+        <v>535</v>
+      </c>
+      <c r="BV8" t="s">
+        <v>536</v>
+      </c>
+      <c r="BW8" t="s">
+        <v>537</v>
+      </c>
+      <c r="BX8" t="s">
+        <v>538</v>
+      </c>
+      <c r="CC8" t="s">
+        <v>539</v>
+      </c>
+      <c r="CD8" t="s">
+        <v>540</v>
+      </c>
+      <c r="CF8" t="s">
+        <v>541</v>
+      </c>
+      <c r="CG8" t="s">
+        <v>542</v>
+      </c>
+      <c r="CI8" t="s">
+        <v>322</v>
+      </c>
+      <c r="CJ8" t="s">
+        <v>543</v>
+      </c>
+      <c r="CL8" t="s">
+        <v>544</v>
+      </c>
+      <c r="CV8" t="s">
+        <v>545</v>
+      </c>
+      <c r="CW8" t="s">
+        <v>546</v>
+      </c>
+      <c r="CX8" t="s">
+        <v>547</v>
+      </c>
+      <c r="CY8" t="s">
+        <v>548</v>
+      </c>
+      <c r="CZ8" t="s">
+        <v>549</v>
+      </c>
+      <c r="DB8" t="s">
+        <v>550</v>
+      </c>
+      <c r="DC8" t="s">
+        <v>551</v>
+      </c>
+      <c r="DD8" t="s">
+        <v>552</v>
+      </c>
+      <c r="DE8" t="s">
+        <v>553</v>
+      </c>
+      <c r="DN8" t="s">
+        <v>142</v>
+      </c>
+      <c r="DR8" t="s">
+        <v>146</v>
+      </c>
+      <c r="DS8" t="s">
+        <v>147</v>
+      </c>
+      <c r="EV8" t="s">
+        <v>174</v>
+      </c>
+      <c r="FE8" t="s">
+        <v>554</v>
+      </c>
+      <c r="GV8" t="s">
+        <v>102</v>
+      </c>
+      <c r="IT8" t="s">
+        <v>236</v>
+      </c>
+      <c r="KY8" t="s">
+        <v>282</v>
+      </c>
+      <c r="LH8" t="s">
+        <v>555</v>
+      </c>
+      <c r="LI8" t="s">
+        <v>556</v>
+      </c>
+      <c r="LN8" t="s">
+        <v>557</v>
+      </c>
+      <c r="LO8" t="s">
+        <v>558</v>
+      </c>
+      <c r="LP8" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>1.0548992723E10</v>
+      </c>
+      <c r="B9">
+        <v>2.26208327E8</v>
+      </c>
+      <c r="C9" s="2">
         <v>43518.46223379629</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <v>43518.56435185186</v>
       </c>
-      <c r="E8" t="s">
-        <v>523</v>
-      </c>
-      <c r="F8" t="s">
-        <v>524</v>
-      </c>
-      <c r="J8" t="s">
-        <v>525</v>
-      </c>
-      <c r="K8" t="s">
-        <v>526</v>
-      </c>
-      <c r="L8" t="s">
-        <v>527</v>
-      </c>
-      <c r="M8" t="s">
-        <v>528</v>
-      </c>
-      <c r="N8" t="s">
-        <v>529</v>
-      </c>
-      <c r="O8" t="s">
-        <v>530</v>
-      </c>
-      <c r="P8" t="s">
-        <v>531</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="E9" t="s">
+        <v>560</v>
+      </c>
+      <c r="F9" t="s">
+        <v>561</v>
+      </c>
+      <c r="J9" t="s">
+        <v>562</v>
+      </c>
+      <c r="K9" t="s">
+        <v>563</v>
+      </c>
+      <c r="L9" t="s">
+        <v>564</v>
+      </c>
+      <c r="M9" t="s">
+        <v>565</v>
+      </c>
+      <c r="N9" t="s">
+        <v>566</v>
+      </c>
+      <c r="O9" t="s">
+        <v>567</v>
+      </c>
+      <c r="P9" t="s">
+        <v>568</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>569</v>
+      </c>
+      <c r="T9" t="s">
+        <v>570</v>
+      </c>
+      <c r="U9" t="s">
+        <v>571</v>
+      </c>
+      <c r="V9" t="s">
+        <v>392</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>305</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>572</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>573</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>574</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>575</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>576</v>
+      </c>
+      <c r="AT9" t="s">
         <v>532</v>
       </c>
-      <c r="T8" t="s">
+      <c r="AU9" t="s">
         <v>533</v>
       </c>
-      <c r="U8" t="s">
-        <v>534</v>
-      </c>
-      <c r="V8" t="s">
-        <v>353</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>535</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>302</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>536</v>
-      </c>
-      <c r="AP8" t="s">
-        <v>537</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>538</v>
-      </c>
-      <c r="AR8" t="s">
-        <v>539</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>495</v>
-      </c>
-      <c r="AV8" t="s">
-        <v>496</v>
-      </c>
-      <c r="BZ8" t="s">
-        <v>540</v>
-      </c>
-      <c r="CC8" t="s">
-        <v>541</v>
-      </c>
-      <c r="CF8" t="s">
-        <v>327</v>
-      </c>
-      <c r="CI8" t="s">
-        <v>542</v>
-      </c>
-      <c r="CL8" t="s">
-        <v>543</v>
-      </c>
-      <c r="CT8" t="s">
-        <v>544</v>
-      </c>
-      <c r="DS8" t="s">
-        <v>99</v>
-      </c>
-      <c r="EQ8" t="s">
-        <v>169</v>
-      </c>
-      <c r="GS8" t="s">
-        <v>99</v>
-      </c>
-      <c r="IT8" t="s">
-        <v>99</v>
-      </c>
-      <c r="KW8" t="s">
-        <v>280</v>
-      </c>
-      <c r="LK8" t="s">
-        <v>545</v>
-      </c>
-      <c r="LM8" t="s">
-        <v>546</v>
+      <c r="CC9" t="s">
+        <v>577</v>
+      </c>
+      <c r="CF9" t="s">
+        <v>578</v>
+      </c>
+      <c r="CI9" t="s">
+        <v>322</v>
+      </c>
+      <c r="CL9" t="s">
+        <v>579</v>
+      </c>
+      <c r="CO9" t="s">
+        <v>580</v>
+      </c>
+      <c r="CW9" t="s">
+        <v>581</v>
+      </c>
+      <c r="DV9" t="s">
+        <v>102</v>
+      </c>
+      <c r="ET9" t="s">
+        <v>172</v>
+      </c>
+      <c r="GV9" t="s">
+        <v>102</v>
+      </c>
+      <c r="IW9" t="s">
+        <v>102</v>
+      </c>
+      <c r="KZ9" t="s">
+        <v>283</v>
+      </c>
+      <c r="LN9" t="s">
+        <v>582</v>
+      </c>
+      <c r="LP9" t="s">
+        <v>583</v>
       </c>
     </row>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
     <row r="15" ht="15.75" customHeight="1"/>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
@@ -5734,10 +6013,6 @@
     <row r="988" ht="15.75" customHeight="1"/>
     <row r="989" ht="15.75" customHeight="1"/>
     <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>

</xml_diff>

<commit_message>
DM-533: [DM-542, DM-543, DM-544] fix bulk importer
+ add colorizing for debugging
+ add choice to destroy practice and re-import
+ update schema
+ fix training details import
+ fix practice permissions import
+ fix IT department import
</commit_message>
<xml_diff>
--- a/lib/assets/Diffusion Marketplace.back.xlsx
+++ b/lib/assets/Diffusion Marketplace.back.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="655">
   <si>
     <t>Respondent ID</t>
   </si>
@@ -61,7 +61,7 @@
     <t>When was this practice initiated? If day is unknown, use the first of the month</t>
   </si>
   <si>
-    <t>Please list the station id of the facility that initiated this Practice. Please reference: https://www.va.gov/directory/guide/rpt_fac_list.cfm?sort=Sta&amp;list_by=all&amp;oid=all</t>
+    <t>Please provide the "facility id" of the facility that initiated this Practice.</t>
   </si>
   <si>
     <t>Please identify where your practice falls currently in VHA’s Phase Gate Model of Innovation.</t>
@@ -999,6 +999,9 @@
     <t>02/01/2012</t>
   </si>
   <si>
+    <t>vha_558</t>
+  </si>
+  <si>
     <t>2. Initial Diffusion - The practice is undergoing active spread to other facilities with a footprint of less than 20% of all VA facilities or other defined target market.</t>
   </si>
   <si>
@@ -1167,6 +1170,9 @@
     <t>09/01/2014</t>
   </si>
   <si>
+    <t>vha_554QB</t>
+  </si>
+  <si>
     <t>3. National Diffusion - Endorsed by a national program office for national dissemination and/or has been implemented at greater than 20% of VA facilities or other defined target market.</t>
   </si>
   <si>
@@ -1230,7 +1236,10 @@
     <t>06/01/2018</t>
   </si>
   <si>
-    <t>Pay for Success project in VACO.</t>
+    <t>vha_679</t>
+  </si>
+  <si>
+    <t>Pay for Success project in VACO</t>
   </si>
   <si>
     <t>Lack of support within the PTSD treatment team to adopt IPS.</t>
@@ -1374,6 +1383,9 @@
     <t>03/28/2013</t>
   </si>
   <si>
+    <t>vha_607</t>
+  </si>
+  <si>
     <t>Longer than one year</t>
   </si>
   <si>
@@ -1398,6 +1410,9 @@
     <t>3. Significant complexity</t>
   </si>
   <si>
+    <t>3. Three departments</t>
+  </si>
+  <si>
     <t>Writer-Editor (GS9)</t>
   </si>
   <si>
@@ -1542,13 +1557,7 @@
     <t>12/01/2010</t>
   </si>
   <si>
-    <t>636A8</t>
-  </si>
-  <si>
-    <t>33 have succesfully implemented the program, 30 current VAMCs offering the Home-based Cardiac Rehab Program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 facilities ( 3 of these were succesful sites up and running and had to close down to do lack of funding) </t>
+    <t>vha_636QJ</t>
   </si>
   <si>
     <t xml:space="preserve">Risk of the implementation not being successfully started due staffing issues. </t>
@@ -1686,7 +1695,7 @@
     <t>01/01/2015</t>
   </si>
   <si>
-    <t>Central Arkansas Veterans Healthcare System, Eugene J. Towbin Healthcare Center (Little Rock, Arkansas)</t>
+    <t>vha_598A0</t>
   </si>
   <si>
     <t>Lack of buy -in</t>
@@ -1737,9 +1746,6 @@
     <t>VIONE@va.gov</t>
   </si>
   <si>
-    <t>Family Medicine\Internal Medicine\Emergency Medicine\please add these 3 to the above list!  Thanks!</t>
-  </si>
-  <si>
     <t>pills_1000x550-730x402.png</t>
   </si>
   <si>
@@ -1779,10 +1785,10 @@
     <t>02/22/2019</t>
   </si>
   <si>
-    <t xml:space="preserve">Puget Sound Health Care System </t>
-  </si>
-  <si>
-    <t>Assemble team and choose a practice chamption</t>
+    <t>vc_0508V</t>
+  </si>
+  <si>
+    <t>Assemble team and choose a Practice Champion</t>
   </si>
   <si>
     <t>1 month</t>
@@ -1938,7 +1944,7 @@
     <t>10/01/2016</t>
   </si>
   <si>
-    <t>Salem VA Medical Center</t>
+    <t>vha_658</t>
   </si>
   <si>
     <t>Office of Nursing Services\VA Dentistry</t>
@@ -1957,9 +1963,6 @@
   </si>
   <si>
     <t>At most $300 for oral care supplies, no development or sustainment cost</t>
-  </si>
-  <si>
-    <t>Some change management and system redesign to operationalize</t>
   </si>
   <si>
     <t>Project HAPPEN started at the Salem VAMC (Salem, VA) and has been replicated at the Michael E. DeBakey VAMC (Houston, TX) through facilitated implementation with the Diffusion of Excellence. It is currently being implemented across VISN 6 Community Living Center (CLC) and medical-surgical inpatient units. @@ -3668,7 +3671,7 @@
         <v>43581.38877314814</v>
       </c>
       <c r="D3" s="2">
-        <v>43586.49127314815</v>
+        <v>43591.90318287037</v>
       </c>
       <c r="E3" t="s">
         <v>317</v>
@@ -3706,11 +3709,11 @@
       <c r="T3" t="s">
         <v>327</v>
       </c>
-      <c r="U3">
-        <v>558.0</v>
+      <c r="U3" t="s">
+        <v>328</v>
       </c>
       <c r="V3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="W3">
         <v>18.0</v>
@@ -3719,7 +3722,7 @@
         <v>2.0</v>
       </c>
       <c r="Y3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AP3" t="s">
         <v>110</v>
@@ -3728,109 +3731,109 @@
         <v>113</v>
       </c>
       <c r="BA3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="BB3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="BC3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="BH3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BI3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BJ3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BK3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BL3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BM3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="BN3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="BO3" t="s">
+        <v>340</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>341</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>341</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>342</v>
+      </c>
+      <c r="CH3" t="s">
         <v>339</v>
       </c>
-      <c r="BX3" t="s">
-        <v>340</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>340</v>
-      </c>
-      <c r="CC3" t="s">
-        <v>341</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>338</v>
-      </c>
       <c r="CI3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CN3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CO3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CP3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CW3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DD3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="DE3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="DF3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="DG3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="DI3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="DJ3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="DL3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="DM3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="DO3" t="s">
         <v>319</v>
       </c>
       <c r="DP3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="DQ3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="DR3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="DU3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="DV3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="DW3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="DZ3" t="s">
         <v>157</v>
@@ -3845,13 +3848,13 @@
         <v>168</v>
       </c>
       <c r="EQ3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="FX3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="GU3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="HH3" t="s">
         <v>119</v>
@@ -3878,28 +3881,28 @@
         <v>307</v>
       </c>
       <c r="MB3" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="MC3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="MI3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="MK3" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="ML3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="MM3" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="MQ3" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="MR3" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4">
@@ -3913,52 +3916,52 @@
         <v>43579.55611111111</v>
       </c>
       <c r="D4" s="2">
-        <v>43584.57293981482</v>
+        <v>43591.91862268518</v>
       </c>
       <c r="E4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="J4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="K4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="M4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="N4" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="O4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="P4" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="Q4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="R4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="S4" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="T4" t="s">
-        <v>383</v>
-      </c>
-      <c r="U4">
-        <v>554.0</v>
+        <v>384</v>
+      </c>
+      <c r="U4" t="s">
+        <v>385</v>
       </c>
       <c r="V4" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="W4">
         <v>11.0</v>
@@ -3967,73 +3970,73 @@
         <v>1.0</v>
       </c>
       <c r="Y4" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AO4" t="s">
         <v>109</v>
       </c>
       <c r="BB4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="BC4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="BD4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="BE4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="BF4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="BG4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="BH4" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="BI4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BJ4" t="s">
+        <v>389</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>390</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>337</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>391</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>392</v>
+      </c>
+      <c r="BS4" t="s">
+        <v>393</v>
+      </c>
+      <c r="BX4" t="s">
+        <v>394</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>395</v>
+      </c>
+      <c r="CD4" t="s">
+        <v>396</v>
+      </c>
+      <c r="CH4" t="s">
+        <v>397</v>
+      </c>
+      <c r="CI4" t="s">
+        <v>392</v>
+      </c>
+      <c r="CW4" t="s">
+        <v>347</v>
+      </c>
+      <c r="DP4" t="s">
         <v>387</v>
-      </c>
-      <c r="BK4" t="s">
-        <v>388</v>
-      </c>
-      <c r="BL4" t="s">
-        <v>336</v>
-      </c>
-      <c r="BM4" t="s">
-        <v>389</v>
-      </c>
-      <c r="BN4" t="s">
-        <v>390</v>
-      </c>
-      <c r="BS4" t="s">
-        <v>391</v>
-      </c>
-      <c r="BX4" t="s">
-        <v>392</v>
-      </c>
-      <c r="CC4" t="s">
-        <v>393</v>
-      </c>
-      <c r="CD4" t="s">
-        <v>394</v>
-      </c>
-      <c r="CH4" t="s">
-        <v>395</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>390</v>
-      </c>
-      <c r="CW4" t="s">
-        <v>346</v>
-      </c>
-      <c r="DP4" t="s">
-        <v>385</v>
       </c>
       <c r="DZ4" t="s">
         <v>157</v>
@@ -4086,43 +4089,43 @@
         <v>43556.49988425926</v>
       </c>
       <c r="D5" s="2">
-        <v>43557.88546296296</v>
+        <v>43591.92634259259</v>
       </c>
       <c r="E5" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F5" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="J5" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="K5" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="L5" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="M5" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="N5" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="O5" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="P5" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="T5" t="s">
-        <v>404</v>
-      </c>
-      <c r="U5">
-        <v>679.0</v>
+        <v>406</v>
+      </c>
+      <c r="U5" t="s">
+        <v>407</v>
       </c>
       <c r="V5" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="W5">
         <v>4.0</v>
@@ -4131,7 +4134,7 @@
         <v>0.0</v>
       </c>
       <c r="Y5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AR5" t="s">
         <v>112</v>
@@ -4140,46 +4143,58 @@
         <v>113</v>
       </c>
       <c r="BA5" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="BB5" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="BC5" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="BD5" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="BE5" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="BF5" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="BG5" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="BH5" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="BI5" t="s">
-        <v>334</v>
+        <v>335</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>335</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>336</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>338</v>
       </c>
       <c r="BN5" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="BO5" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="BP5" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="BQ5" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="BR5" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="BS5">
         <v>2.0</v>
@@ -4197,85 +4212,85 @@
         <v>40.0</v>
       </c>
       <c r="BX5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="BY5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="BZ5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="CA5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="CB5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="CC5" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="CD5" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="CE5" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="CH5" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="CI5" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="CJ5" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="CK5" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="CL5" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="CM5" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="CN5" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="CO5" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="CP5" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="CQ5" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="CW5" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DC5" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="DD5" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="DE5" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="DG5" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="DH5" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="DO5" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="DP5" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="DQ5" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="DZ5" t="s">
         <v>157</v>
@@ -4302,13 +4317,13 @@
         <v>119</v>
       </c>
       <c r="HQ5" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="JC5" t="s">
         <v>250</v>
       </c>
       <c r="JR5" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="LD5" t="s">
         <v>295</v>
@@ -4320,22 +4335,22 @@
         <v>304</v>
       </c>
       <c r="MA5" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="MC5" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="MF5" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="ML5" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="MM5" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="MS5" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="6">
@@ -4349,49 +4364,49 @@
         <v>43556.35381944444</v>
       </c>
       <c r="D6" s="2">
-        <v>43557.57269675926</v>
+        <v>43591.92844907408</v>
       </c>
       <c r="E6" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="F6" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="J6" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="K6" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="L6" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="M6" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="N6" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="O6" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="P6" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="Q6" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="R6" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="T6" t="s">
-        <v>452</v>
-      </c>
-      <c r="U6">
-        <v>607.0</v>
+        <v>455</v>
+      </c>
+      <c r="U6" t="s">
+        <v>456</v>
       </c>
       <c r="V6" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="W6">
         <v>21.0</v>
@@ -4400,7 +4415,7 @@
         <v>3.0</v>
       </c>
       <c r="Y6" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="AP6" t="s">
         <v>110</v>
@@ -4412,124 +4427,136 @@
         <v>120</v>
       </c>
       <c r="BB6" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="BC6" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="BD6" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="BE6" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="BF6" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="BG6" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="BH6" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BI6" t="s">
-        <v>460</v>
+        <v>464</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>464</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>465</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM6" t="s">
+        <v>338</v>
       </c>
       <c r="BN6" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="BS6" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="BX6" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="CC6" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="CH6" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="CI6" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="CJ6" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="CK6" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="CL6" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="CM6" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="CN6" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="CP6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CW6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DC6" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="DD6" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="DE6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="DF6" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="DG6" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="DH6" t="s">
+        <v>478</v>
+      </c>
+      <c r="DI6" t="s">
+        <v>479</v>
+      </c>
+      <c r="DJ6" t="s">
+        <v>480</v>
+      </c>
+      <c r="DK6" t="s">
+        <v>481</v>
+      </c>
+      <c r="DL6" t="s">
+        <v>482</v>
+      </c>
+      <c r="DM6" t="s">
+        <v>483</v>
+      </c>
+      <c r="DN6" t="s">
+        <v>484</v>
+      </c>
+      <c r="DO6" t="s">
+        <v>485</v>
+      </c>
+      <c r="DP6" t="s">
+        <v>486</v>
+      </c>
+      <c r="DQ6" t="s">
+        <v>487</v>
+      </c>
+      <c r="DR6" t="s">
+        <v>488</v>
+      </c>
+      <c r="DU6" t="s">
         <v>473</v>
       </c>
-      <c r="DI6" t="s">
-        <v>474</v>
-      </c>
-      <c r="DJ6" t="s">
-        <v>475</v>
-      </c>
-      <c r="DK6" t="s">
-        <v>476</v>
-      </c>
-      <c r="DL6" t="s">
-        <v>477</v>
-      </c>
-      <c r="DM6" t="s">
-        <v>478</v>
-      </c>
-      <c r="DN6" t="s">
-        <v>479</v>
-      </c>
-      <c r="DO6" t="s">
-        <v>480</v>
-      </c>
-      <c r="DP6" t="s">
-        <v>481</v>
-      </c>
-      <c r="DQ6" t="s">
-        <v>482</v>
-      </c>
-      <c r="DR6" t="s">
-        <v>483</v>
-      </c>
-      <c r="DU6" t="s">
-        <v>468</v>
-      </c>
       <c r="DV6" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="DW6" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="DZ6" t="s">
         <v>157</v>
@@ -4685,7 +4712,7 @@
         <v>213</v>
       </c>
       <c r="HQ6" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="JG6" t="s">
         <v>253</v>
@@ -4778,34 +4805,34 @@
         <v>310</v>
       </c>
       <c r="MB6" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="MC6" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="MF6" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="MG6" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="MH6" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="MI6" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="MK6" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
       <c r="ML6" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="MN6" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="MS6" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
     </row>
     <row r="7">
@@ -4819,88 +4846,100 @@
         <v>43552.51997685185</v>
       </c>
       <c r="D7" s="2">
-        <v>43557.43107638889</v>
+        <v>43591.93149305556</v>
       </c>
       <c r="E7" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="F7" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="J7" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="K7" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="L7" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="M7" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="N7" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="O7" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="P7" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="Q7" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="R7" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="T7" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="U7" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="V7" t="s">
-        <v>328</v>
-      </c>
-      <c r="W7" t="s">
-        <v>510</v>
-      </c>
-      <c r="X7" t="s">
-        <v>511</v>
+        <v>329</v>
+      </c>
+      <c r="W7">
+        <v>33.0</v>
+      </c>
+      <c r="X7">
+        <v>6.0</v>
       </c>
       <c r="Y7" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="AO7" t="s">
         <v>109</v>
       </c>
       <c r="BB7" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="BC7" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="BD7" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="BE7" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="BH7" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="BI7" t="s">
-        <v>334</v>
+        <v>335</v>
+      </c>
+      <c r="BJ7" t="s">
+        <v>389</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>390</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM7" t="s">
+        <v>338</v>
       </c>
       <c r="BN7" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="BO7" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="BP7" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="BS7">
         <v>40.0</v>
@@ -4909,70 +4948,70 @@
         <v>5.0</v>
       </c>
       <c r="BU7" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="BX7" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="BY7" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="BZ7" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="CC7" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="CD7" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="CH7" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="CI7" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="CJ7" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="CN7" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="CO7" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="CP7" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="CW7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DC7" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="DD7" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="DE7" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="DO7" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="DP7" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="DQ7" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="DR7" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="DS7" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="DT7" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="DZ7" t="s">
         <v>157</v>
@@ -5008,19 +5047,19 @@
         <v>119</v>
       </c>
       <c r="HR7" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="HS7" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="HT7" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="HU7" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="HV7" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="IE7" t="s">
         <v>227</v>
@@ -5068,22 +5107,22 @@
         <v>306</v>
       </c>
       <c r="MA7" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="MC7" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="MK7" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="ML7" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="MN7" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="MT7" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
     </row>
     <row r="8">
@@ -5097,73 +5136,85 @@
         <v>43520.39091435185</v>
       </c>
       <c r="D8" s="2">
-        <v>43532.62158564815</v>
+        <v>43591.9340625</v>
       </c>
       <c r="E8" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="J8" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="K8" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="L8" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="M8" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="N8" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="O8" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="P8" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="Q8" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="R8" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="T8" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="U8" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="V8" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="Y8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AP8" t="s">
         <v>110</v>
       </c>
       <c r="BB8" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="BC8" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="BD8" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="BE8" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="BH8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BI8" t="s">
-        <v>334</v>
+        <v>335</v>
+      </c>
+      <c r="BJ8" t="s">
+        <v>389</v>
+      </c>
+      <c r="BK8" t="s">
+        <v>390</v>
+      </c>
+      <c r="BL8" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM8" t="s">
+        <v>338</v>
       </c>
       <c r="BN8" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="BO8" t="s">
         <v>309</v>
@@ -5181,55 +5232,52 @@
         <v>52.0</v>
       </c>
       <c r="CC8" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="CD8" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="CH8" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="CI8" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="CJ8" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="CQ8" t="s">
-        <v>568</v>
-      </c>
-      <c r="CT8" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="CW8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DD8" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="DE8" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="DG8" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="DH8" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="DO8" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="DP8" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="DR8" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="DS8" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="DT8" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="EG8" t="s">
         <v>164</v>
@@ -5252,11 +5300,20 @@
       <c r="EN8" t="s">
         <v>171</v>
       </c>
-      <c r="FT8" t="s">
-        <v>201</v>
-      </c>
-      <c r="FX8" t="s">
-        <v>574</v>
+      <c r="ES8" t="s">
+        <v>174</v>
+      </c>
+      <c r="ET8" t="s">
+        <v>175</v>
+      </c>
+      <c r="EW8" t="s">
+        <v>178</v>
+      </c>
+      <c r="GT8" t="s">
+        <v>119</v>
+      </c>
+      <c r="HH8" t="s">
+        <v>119</v>
       </c>
       <c r="HO8" t="s">
         <v>119</v>
@@ -5289,10 +5346,10 @@
         <v>309</v>
       </c>
       <c r="MB8" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="MT8" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="9">
@@ -5306,163 +5363,163 @@
         <v>43518.48881944444</v>
       </c>
       <c r="D9" s="2">
-        <v>43590.96472222222</v>
+        <v>43591.94086805556</v>
       </c>
       <c r="E9" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="F9" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="J9" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="K9" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="L9" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="M9" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="N9" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="O9" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="P9" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="Q9" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="T9" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="U9" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="V9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="Y9" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AA9" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="AB9" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="AC9" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="AD9" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="AE9" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="AF9" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="AG9" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="AH9" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="AP9" t="s">
         <v>110</v>
       </c>
       <c r="BA9" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="BB9" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="BC9" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="BH9" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="BI9" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="BJ9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BK9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BL9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BM9" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CH9" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="CI9" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="CJ9" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="CK9" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="CL9" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="CQ9" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="CR9" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="CW9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DC9" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="DD9" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="DE9" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="DO9" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="DP9" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="DQ9" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="DR9" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="DS9" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="DU9" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="DV9" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="DW9" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="DX9" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="DZ9" t="s">
         <v>157</v>
@@ -5480,7 +5537,7 @@
         <v>169</v>
       </c>
       <c r="FX9" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="GM9" t="s">
         <v>196</v>
@@ -5510,31 +5567,31 @@
         <v>304</v>
       </c>
       <c r="MA9" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="MB9" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="MC9" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="MD9" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="ME9" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="MF9" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="MI9" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="MJ9" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="MK9" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="10">
@@ -5548,109 +5605,133 @@
         <v>43518.46223379629</v>
       </c>
       <c r="D10" s="2">
-        <v>43585.3855787037</v>
+        <v>43591.90581018518</v>
       </c>
       <c r="E10" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="F10" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="J10" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="K10" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="L10" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="M10" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="N10" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="O10" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="P10" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="Q10" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="T10" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="U10" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="V10" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="Y10" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="BA10" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="BB10" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="BC10" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="BD10" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="BE10" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="BH10" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="BI10" t="s">
-        <v>600</v>
+        <v>602</v>
+      </c>
+      <c r="BJ10" t="s">
+        <v>389</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>390</v>
+      </c>
+      <c r="BL10" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM10" t="s">
+        <v>338</v>
       </c>
       <c r="CQ10" t="s">
-        <v>647</v>
-      </c>
-      <c r="CT10" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="CW10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DE10" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="DH10" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="DP10" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="EO10" t="s">
         <v>119</v>
       </c>
-      <c r="FM10" t="s">
-        <v>194</v>
+      <c r="FL10" t="s">
+        <v>193</v>
+      </c>
+      <c r="GM10" t="s">
+        <v>196</v>
+      </c>
+      <c r="HH10" t="s">
+        <v>119</v>
       </c>
       <c r="HO10" t="s">
         <v>119</v>
       </c>
+      <c r="JB10" t="s">
+        <v>249</v>
+      </c>
+      <c r="JC10" t="s">
+        <v>250</v>
+      </c>
       <c r="JP10" t="s">
         <v>119</v>
       </c>
+      <c r="KE10" t="s">
+        <v>274</v>
+      </c>
       <c r="LS10" t="s">
         <v>305</v>
       </c>
       <c r="MI10" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="MK10" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
DM-533: [DM-542, DM-543, DM-544] fix bulk importer (#41)
+ add colorizing for debugging
+ add choice to destroy practice and re-import
+ update schema
+ fix training details import
+ fix practice permissions import
+ fix IT department import
</commit_message>
<xml_diff>
--- a/lib/assets/Diffusion Marketplace.back.xlsx
+++ b/lib/assets/Diffusion Marketplace.back.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="655">
   <si>
     <t>Respondent ID</t>
   </si>
@@ -61,7 +61,7 @@
     <t>When was this practice initiated? If day is unknown, use the first of the month</t>
   </si>
   <si>
-    <t>Please list the station id of the facility that initiated this Practice. Please reference: https://www.va.gov/directory/guide/rpt_fac_list.cfm?sort=Sta&amp;list_by=all&amp;oid=all</t>
+    <t>Please provide the "facility id" of the facility that initiated this Practice.</t>
   </si>
   <si>
     <t>Please identify where your practice falls currently in VHA’s Phase Gate Model of Innovation.</t>
@@ -999,6 +999,9 @@
     <t>02/01/2012</t>
   </si>
   <si>
+    <t>vha_558</t>
+  </si>
+  <si>
     <t>2. Initial Diffusion - The practice is undergoing active spread to other facilities with a footprint of less than 20% of all VA facilities or other defined target market.</t>
   </si>
   <si>
@@ -1167,6 +1170,9 @@
     <t>09/01/2014</t>
   </si>
   <si>
+    <t>vha_554QB</t>
+  </si>
+  <si>
     <t>3. National Diffusion - Endorsed by a national program office for national dissemination and/or has been implemented at greater than 20% of VA facilities or other defined target market.</t>
   </si>
   <si>
@@ -1230,7 +1236,10 @@
     <t>06/01/2018</t>
   </si>
   <si>
-    <t>Pay for Success project in VACO.</t>
+    <t>vha_679</t>
+  </si>
+  <si>
+    <t>Pay for Success project in VACO</t>
   </si>
   <si>
     <t>Lack of support within the PTSD treatment team to adopt IPS.</t>
@@ -1374,6 +1383,9 @@
     <t>03/28/2013</t>
   </si>
   <si>
+    <t>vha_607</t>
+  </si>
+  <si>
     <t>Longer than one year</t>
   </si>
   <si>
@@ -1398,6 +1410,9 @@
     <t>3. Significant complexity</t>
   </si>
   <si>
+    <t>3. Three departments</t>
+  </si>
+  <si>
     <t>Writer-Editor (GS9)</t>
   </si>
   <si>
@@ -1542,13 +1557,7 @@
     <t>12/01/2010</t>
   </si>
   <si>
-    <t>636A8</t>
-  </si>
-  <si>
-    <t>33 have succesfully implemented the program, 30 current VAMCs offering the Home-based Cardiac Rehab Program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 facilities ( 3 of these were succesful sites up and running and had to close down to do lack of funding) </t>
+    <t>vha_636QJ</t>
   </si>
   <si>
     <t xml:space="preserve">Risk of the implementation not being successfully started due staffing issues. </t>
@@ -1686,7 +1695,7 @@
     <t>01/01/2015</t>
   </si>
   <si>
-    <t>Central Arkansas Veterans Healthcare System, Eugene J. Towbin Healthcare Center (Little Rock, Arkansas)</t>
+    <t>vha_598A0</t>
   </si>
   <si>
     <t>Lack of buy -in</t>
@@ -1737,9 +1746,6 @@
     <t>VIONE@va.gov</t>
   </si>
   <si>
-    <t>Family Medicine\Internal Medicine\Emergency Medicine\please add these 3 to the above list!  Thanks!</t>
-  </si>
-  <si>
     <t>pills_1000x550-730x402.png</t>
   </si>
   <si>
@@ -1779,10 +1785,10 @@
     <t>02/22/2019</t>
   </si>
   <si>
-    <t xml:space="preserve">Puget Sound Health Care System </t>
-  </si>
-  <si>
-    <t>Assemble team and choose a practice chamption</t>
+    <t>vc_0508V</t>
+  </si>
+  <si>
+    <t>Assemble team and choose a Practice Champion</t>
   </si>
   <si>
     <t>1 month</t>
@@ -1938,7 +1944,7 @@
     <t>10/01/2016</t>
   </si>
   <si>
-    <t>Salem VA Medical Center</t>
+    <t>vha_658</t>
   </si>
   <si>
     <t>Office of Nursing Services\VA Dentistry</t>
@@ -1957,9 +1963,6 @@
   </si>
   <si>
     <t>At most $300 for oral care supplies, no development or sustainment cost</t>
-  </si>
-  <si>
-    <t>Some change management and system redesign to operationalize</t>
   </si>
   <si>
     <t>Project HAPPEN started at the Salem VAMC (Salem, VA) and has been replicated at the Michael E. DeBakey VAMC (Houston, TX) through facilitated implementation with the Diffusion of Excellence. It is currently being implemented across VISN 6 Community Living Center (CLC) and medical-surgical inpatient units. @@ -3668,7 +3671,7 @@
         <v>43581.38877314814</v>
       </c>
       <c r="D3" s="2">
-        <v>43586.49127314815</v>
+        <v>43591.90318287037</v>
       </c>
       <c r="E3" t="s">
         <v>317</v>
@@ -3706,11 +3709,11 @@
       <c r="T3" t="s">
         <v>327</v>
       </c>
-      <c r="U3">
-        <v>558.0</v>
+      <c r="U3" t="s">
+        <v>328</v>
       </c>
       <c r="V3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="W3">
         <v>18.0</v>
@@ -3719,7 +3722,7 @@
         <v>2.0</v>
       </c>
       <c r="Y3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AP3" t="s">
         <v>110</v>
@@ -3728,109 +3731,109 @@
         <v>113</v>
       </c>
       <c r="BA3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="BB3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="BC3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="BH3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BI3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BJ3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BK3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BL3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BM3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="BN3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="BO3" t="s">
+        <v>340</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>341</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>341</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>342</v>
+      </c>
+      <c r="CH3" t="s">
         <v>339</v>
       </c>
-      <c r="BX3" t="s">
-        <v>340</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>340</v>
-      </c>
-      <c r="CC3" t="s">
-        <v>341</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>338</v>
-      </c>
       <c r="CI3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CN3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CO3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CP3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CW3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DD3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="DE3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="DF3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="DG3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="DI3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="DJ3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="DL3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="DM3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="DO3" t="s">
         <v>319</v>
       </c>
       <c r="DP3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="DQ3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="DR3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="DU3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="DV3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="DW3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="DZ3" t="s">
         <v>157</v>
@@ -3845,13 +3848,13 @@
         <v>168</v>
       </c>
       <c r="EQ3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="FX3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="GU3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="HH3" t="s">
         <v>119</v>
@@ -3878,28 +3881,28 @@
         <v>307</v>
       </c>
       <c r="MB3" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="MC3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="MI3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="MK3" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="ML3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="MM3" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="MQ3" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="MR3" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4">
@@ -3913,52 +3916,52 @@
         <v>43579.55611111111</v>
       </c>
       <c r="D4" s="2">
-        <v>43584.57293981482</v>
+        <v>43591.91862268518</v>
       </c>
       <c r="E4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="J4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="K4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="M4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="N4" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="O4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="P4" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="Q4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="R4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="S4" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="T4" t="s">
-        <v>383</v>
-      </c>
-      <c r="U4">
-        <v>554.0</v>
+        <v>384</v>
+      </c>
+      <c r="U4" t="s">
+        <v>385</v>
       </c>
       <c r="V4" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="W4">
         <v>11.0</v>
@@ -3967,73 +3970,73 @@
         <v>1.0</v>
       </c>
       <c r="Y4" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AO4" t="s">
         <v>109</v>
       </c>
       <c r="BB4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="BC4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="BD4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="BE4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="BF4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="BG4" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="BH4" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="BI4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BJ4" t="s">
+        <v>389</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>390</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>337</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>391</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>392</v>
+      </c>
+      <c r="BS4" t="s">
+        <v>393</v>
+      </c>
+      <c r="BX4" t="s">
+        <v>394</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>395</v>
+      </c>
+      <c r="CD4" t="s">
+        <v>396</v>
+      </c>
+      <c r="CH4" t="s">
+        <v>397</v>
+      </c>
+      <c r="CI4" t="s">
+        <v>392</v>
+      </c>
+      <c r="CW4" t="s">
+        <v>347</v>
+      </c>
+      <c r="DP4" t="s">
         <v>387</v>
-      </c>
-      <c r="BK4" t="s">
-        <v>388</v>
-      </c>
-      <c r="BL4" t="s">
-        <v>336</v>
-      </c>
-      <c r="BM4" t="s">
-        <v>389</v>
-      </c>
-      <c r="BN4" t="s">
-        <v>390</v>
-      </c>
-      <c r="BS4" t="s">
-        <v>391</v>
-      </c>
-      <c r="BX4" t="s">
-        <v>392</v>
-      </c>
-      <c r="CC4" t="s">
-        <v>393</v>
-      </c>
-      <c r="CD4" t="s">
-        <v>394</v>
-      </c>
-      <c r="CH4" t="s">
-        <v>395</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>390</v>
-      </c>
-      <c r="CW4" t="s">
-        <v>346</v>
-      </c>
-      <c r="DP4" t="s">
-        <v>385</v>
       </c>
       <c r="DZ4" t="s">
         <v>157</v>
@@ -4086,43 +4089,43 @@
         <v>43556.49988425926</v>
       </c>
       <c r="D5" s="2">
-        <v>43557.88546296296</v>
+        <v>43591.92634259259</v>
       </c>
       <c r="E5" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="F5" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="J5" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="K5" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="L5" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="M5" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="N5" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="O5" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="P5" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="T5" t="s">
-        <v>404</v>
-      </c>
-      <c r="U5">
-        <v>679.0</v>
+        <v>406</v>
+      </c>
+      <c r="U5" t="s">
+        <v>407</v>
       </c>
       <c r="V5" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="W5">
         <v>4.0</v>
@@ -4131,7 +4134,7 @@
         <v>0.0</v>
       </c>
       <c r="Y5" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AR5" t="s">
         <v>112</v>
@@ -4140,46 +4143,58 @@
         <v>113</v>
       </c>
       <c r="BA5" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="BB5" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="BC5" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="BD5" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="BE5" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="BF5" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="BG5" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="BH5" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="BI5" t="s">
-        <v>334</v>
+        <v>335</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>335</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>336</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>338</v>
       </c>
       <c r="BN5" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="BO5" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="BP5" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="BQ5" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="BR5" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="BS5">
         <v>2.0</v>
@@ -4197,85 +4212,85 @@
         <v>40.0</v>
       </c>
       <c r="BX5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="BY5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="BZ5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="CA5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="CB5" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="CC5" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="CD5" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="CE5" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="CH5" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="CI5" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="CJ5" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="CK5" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="CL5" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="CM5" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="CN5" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="CO5" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="CP5" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="CQ5" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="CW5" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DC5" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="DD5" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="DE5" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="DG5" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="DH5" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="DO5" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="DP5" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="DQ5" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="DZ5" t="s">
         <v>157</v>
@@ -4302,13 +4317,13 @@
         <v>119</v>
       </c>
       <c r="HQ5" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="JC5" t="s">
         <v>250</v>
       </c>
       <c r="JR5" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="LD5" t="s">
         <v>295</v>
@@ -4320,22 +4335,22 @@
         <v>304</v>
       </c>
       <c r="MA5" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="MC5" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="MF5" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="ML5" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="MM5" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="MS5" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="6">
@@ -4349,49 +4364,49 @@
         <v>43556.35381944444</v>
       </c>
       <c r="D6" s="2">
-        <v>43557.57269675926</v>
+        <v>43591.92844907408</v>
       </c>
       <c r="E6" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="F6" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="J6" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="K6" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="L6" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="M6" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="N6" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="O6" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="P6" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="Q6" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="R6" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="T6" t="s">
-        <v>452</v>
-      </c>
-      <c r="U6">
-        <v>607.0</v>
+        <v>455</v>
+      </c>
+      <c r="U6" t="s">
+        <v>456</v>
       </c>
       <c r="V6" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="W6">
         <v>21.0</v>
@@ -4400,7 +4415,7 @@
         <v>3.0</v>
       </c>
       <c r="Y6" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="AP6" t="s">
         <v>110</v>
@@ -4412,124 +4427,136 @@
         <v>120</v>
       </c>
       <c r="BB6" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="BC6" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="BD6" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="BE6" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="BF6" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="BG6" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="BH6" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BI6" t="s">
-        <v>460</v>
+        <v>464</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>464</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>465</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM6" t="s">
+        <v>338</v>
       </c>
       <c r="BN6" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="BS6" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="BX6" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="CC6" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="CH6" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="CI6" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="CJ6" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="CK6" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="CL6" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="CM6" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="CN6" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="CP6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CW6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DC6" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="DD6" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="DE6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="DF6" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="DG6" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="DH6" t="s">
+        <v>478</v>
+      </c>
+      <c r="DI6" t="s">
+        <v>479</v>
+      </c>
+      <c r="DJ6" t="s">
+        <v>480</v>
+      </c>
+      <c r="DK6" t="s">
+        <v>481</v>
+      </c>
+      <c r="DL6" t="s">
+        <v>482</v>
+      </c>
+      <c r="DM6" t="s">
+        <v>483</v>
+      </c>
+      <c r="DN6" t="s">
+        <v>484</v>
+      </c>
+      <c r="DO6" t="s">
+        <v>485</v>
+      </c>
+      <c r="DP6" t="s">
+        <v>486</v>
+      </c>
+      <c r="DQ6" t="s">
+        <v>487</v>
+      </c>
+      <c r="DR6" t="s">
+        <v>488</v>
+      </c>
+      <c r="DU6" t="s">
         <v>473</v>
       </c>
-      <c r="DI6" t="s">
-        <v>474</v>
-      </c>
-      <c r="DJ6" t="s">
-        <v>475</v>
-      </c>
-      <c r="DK6" t="s">
-        <v>476</v>
-      </c>
-      <c r="DL6" t="s">
-        <v>477</v>
-      </c>
-      <c r="DM6" t="s">
-        <v>478</v>
-      </c>
-      <c r="DN6" t="s">
-        <v>479</v>
-      </c>
-      <c r="DO6" t="s">
-        <v>480</v>
-      </c>
-      <c r="DP6" t="s">
-        <v>481</v>
-      </c>
-      <c r="DQ6" t="s">
-        <v>482</v>
-      </c>
-      <c r="DR6" t="s">
-        <v>483</v>
-      </c>
-      <c r="DU6" t="s">
-        <v>468</v>
-      </c>
       <c r="DV6" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="DW6" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="DZ6" t="s">
         <v>157</v>
@@ -4685,7 +4712,7 @@
         <v>213</v>
       </c>
       <c r="HQ6" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="JG6" t="s">
         <v>253</v>
@@ -4778,34 +4805,34 @@
         <v>310</v>
       </c>
       <c r="MB6" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="MC6" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="MF6" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="MG6" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="MH6" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="MI6" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="MK6" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
       <c r="ML6" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="MN6" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="MS6" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
     </row>
     <row r="7">
@@ -4819,88 +4846,100 @@
         <v>43552.51997685185</v>
       </c>
       <c r="D7" s="2">
-        <v>43557.43107638889</v>
+        <v>43591.93149305556</v>
       </c>
       <c r="E7" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="F7" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="J7" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="K7" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="L7" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="M7" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="N7" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="O7" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="P7" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="Q7" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="R7" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="T7" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="U7" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="V7" t="s">
-        <v>328</v>
-      </c>
-      <c r="W7" t="s">
-        <v>510</v>
-      </c>
-      <c r="X7" t="s">
-        <v>511</v>
+        <v>329</v>
+      </c>
+      <c r="W7">
+        <v>33.0</v>
+      </c>
+      <c r="X7">
+        <v>6.0</v>
       </c>
       <c r="Y7" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="AO7" t="s">
         <v>109</v>
       </c>
       <c r="BB7" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="BC7" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="BD7" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="BE7" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="BH7" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="BI7" t="s">
-        <v>334</v>
+        <v>335</v>
+      </c>
+      <c r="BJ7" t="s">
+        <v>389</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>390</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM7" t="s">
+        <v>338</v>
       </c>
       <c r="BN7" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="BO7" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="BP7" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="BS7">
         <v>40.0</v>
@@ -4909,70 +4948,70 @@
         <v>5.0</v>
       </c>
       <c r="BU7" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="BX7" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="BY7" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="BZ7" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="CC7" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="CD7" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="CH7" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="CI7" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="CJ7" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="CN7" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="CO7" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="CP7" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="CW7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DC7" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="DD7" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="DE7" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="DO7" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="DP7" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="DQ7" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="DR7" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="DS7" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="DT7" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="DZ7" t="s">
         <v>157</v>
@@ -5008,19 +5047,19 @@
         <v>119</v>
       </c>
       <c r="HR7" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="HS7" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="HT7" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="HU7" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="HV7" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="IE7" t="s">
         <v>227</v>
@@ -5068,22 +5107,22 @@
         <v>306</v>
       </c>
       <c r="MA7" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="MC7" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="MK7" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="ML7" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="MN7" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="MT7" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
     </row>
     <row r="8">
@@ -5097,73 +5136,85 @@
         <v>43520.39091435185</v>
       </c>
       <c r="D8" s="2">
-        <v>43532.62158564815</v>
+        <v>43591.9340625</v>
       </c>
       <c r="E8" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="J8" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="K8" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="L8" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="M8" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="N8" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="O8" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="P8" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="Q8" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="R8" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="T8" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="U8" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="V8" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="Y8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AP8" t="s">
         <v>110</v>
       </c>
       <c r="BB8" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="BC8" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="BD8" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="BE8" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="BH8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BI8" t="s">
-        <v>334</v>
+        <v>335</v>
+      </c>
+      <c r="BJ8" t="s">
+        <v>389</v>
+      </c>
+      <c r="BK8" t="s">
+        <v>390</v>
+      </c>
+      <c r="BL8" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM8" t="s">
+        <v>338</v>
       </c>
       <c r="BN8" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="BO8" t="s">
         <v>309</v>
@@ -5181,55 +5232,52 @@
         <v>52.0</v>
       </c>
       <c r="CC8" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="CD8" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="CH8" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="CI8" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="CJ8" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="CQ8" t="s">
-        <v>568</v>
-      </c>
-      <c r="CT8" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="CW8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DD8" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="DE8" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="DG8" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="DH8" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="DO8" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="DP8" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="DR8" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="DS8" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="DT8" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="EG8" t="s">
         <v>164</v>
@@ -5252,11 +5300,20 @@
       <c r="EN8" t="s">
         <v>171</v>
       </c>
-      <c r="FT8" t="s">
-        <v>201</v>
-      </c>
-      <c r="FX8" t="s">
-        <v>574</v>
+      <c r="ES8" t="s">
+        <v>174</v>
+      </c>
+      <c r="ET8" t="s">
+        <v>175</v>
+      </c>
+      <c r="EW8" t="s">
+        <v>178</v>
+      </c>
+      <c r="GT8" t="s">
+        <v>119</v>
+      </c>
+      <c r="HH8" t="s">
+        <v>119</v>
       </c>
       <c r="HO8" t="s">
         <v>119</v>
@@ -5289,10 +5346,10 @@
         <v>309</v>
       </c>
       <c r="MB8" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="MT8" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="9">
@@ -5306,163 +5363,163 @@
         <v>43518.48881944444</v>
       </c>
       <c r="D9" s="2">
-        <v>43590.96472222222</v>
+        <v>43591.94086805556</v>
       </c>
       <c r="E9" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="F9" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="J9" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="K9" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="L9" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="M9" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="N9" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="O9" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="P9" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="Q9" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="T9" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="U9" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="V9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="Y9" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AA9" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="AB9" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="AC9" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="AD9" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="AE9" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="AF9" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="AG9" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="AH9" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="AP9" t="s">
         <v>110</v>
       </c>
       <c r="BA9" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="BB9" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="BC9" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="BH9" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="BI9" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="BJ9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BK9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BL9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BM9" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CH9" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="CI9" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="CJ9" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="CK9" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="CL9" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="CQ9" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="CR9" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="CW9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DC9" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="DD9" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="DE9" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="DO9" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="DP9" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="DQ9" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="DR9" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="DS9" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="DU9" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="DV9" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="DW9" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="DX9" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="DZ9" t="s">
         <v>157</v>
@@ -5480,7 +5537,7 @@
         <v>169</v>
       </c>
       <c r="FX9" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="GM9" t="s">
         <v>196</v>
@@ -5510,31 +5567,31 @@
         <v>304</v>
       </c>
       <c r="MA9" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="MB9" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="MC9" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="MD9" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="ME9" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="MF9" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="MI9" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="MJ9" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="MK9" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="10">
@@ -5548,109 +5605,133 @@
         <v>43518.46223379629</v>
       </c>
       <c r="D10" s="2">
-        <v>43585.3855787037</v>
+        <v>43591.90581018518</v>
       </c>
       <c r="E10" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="F10" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="J10" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="K10" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="L10" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="M10" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="N10" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="O10" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="P10" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="Q10" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="T10" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="U10" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="V10" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="Y10" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="BA10" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="BB10" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="BC10" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="BD10" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="BE10" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="BH10" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="BI10" t="s">
-        <v>600</v>
+        <v>602</v>
+      </c>
+      <c r="BJ10" t="s">
+        <v>389</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>390</v>
+      </c>
+      <c r="BL10" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM10" t="s">
+        <v>338</v>
       </c>
       <c r="CQ10" t="s">
-        <v>647</v>
-      </c>
-      <c r="CT10" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="CW10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="DE10" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="DH10" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="DP10" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="EO10" t="s">
         <v>119</v>
       </c>
-      <c r="FM10" t="s">
-        <v>194</v>
+      <c r="FL10" t="s">
+        <v>193</v>
+      </c>
+      <c r="GM10" t="s">
+        <v>196</v>
+      </c>
+      <c r="HH10" t="s">
+        <v>119</v>
       </c>
       <c r="HO10" t="s">
         <v>119</v>
       </c>
+      <c r="JB10" t="s">
+        <v>249</v>
+      </c>
+      <c r="JC10" t="s">
+        <v>250</v>
+      </c>
       <c r="JP10" t="s">
         <v>119</v>
       </c>
+      <c r="KE10" t="s">
+        <v>274</v>
+      </c>
       <c r="LS10" t="s">
         <v>305</v>
       </c>
       <c r="MI10" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="MK10" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1"/>

</xml_diff>